<commit_message>
update existing lb linkages
</commit_message>
<xml_diff>
--- a/result/Foundation Model Leaderboards.xlsx
+++ b/result/Foundation Model Leaderboards.xlsx
@@ -164,7 +164,7 @@
       <text>
         <t xml:space="preserve">https://swahili-llm-leaderboard.streamlit.app
 	-Jimmy Zhao
-https://github.com/msamwelmollel/Swahili_LLM_Leaderboard?tab=readme-ov-file#leaderboard
+https://huggingface.co/spaces/sartifyllc/Swahili_LLM_Leaderboard
 	-Jimmy Zhao</t>
       </text>
     </comment>
@@ -21413,7 +21413,7 @@
     <hyperlink r:id="rId312" ref="A166"/>
     <hyperlink r:id="rId313" ref="C166"/>
     <hyperlink r:id="rId314" ref="I166"/>
-    <hyperlink r:id="rId315" ref="A167"/>
+    <hyperlink r:id="rId315" location="leaderboard" ref="A167"/>
     <hyperlink r:id="rId316" ref="C167"/>
     <hyperlink r:id="rId317" location="leaderboard" ref="A168"/>
     <hyperlink r:id="rId318" ref="C168"/>
@@ -21471,7 +21471,7 @@
     <hyperlink r:id="rId370" ref="C196"/>
     <hyperlink r:id="rId371" ref="A197"/>
     <hyperlink r:id="rId372" ref="C197"/>
-    <hyperlink r:id="rId373" ref="A198"/>
+    <hyperlink r:id="rId373" location="results-preview" ref="A198"/>
     <hyperlink r:id="rId374" ref="C198"/>
     <hyperlink r:id="rId375" ref="A199"/>
     <hyperlink r:id="rId376" ref="C199"/>
@@ -21529,7 +21529,7 @@
     <hyperlink r:id="rId428" ref="I224"/>
     <hyperlink r:id="rId429" ref="A225"/>
     <hyperlink r:id="rId430" ref="C225"/>
-    <hyperlink r:id="rId431" ref="A226"/>
+    <hyperlink r:id="rId431" location="leaderboard" ref="A226"/>
     <hyperlink r:id="rId432" ref="C226"/>
     <hyperlink r:id="rId433" ref="I226"/>
     <hyperlink r:id="rId434" ref="A227"/>
@@ -21962,7 +21962,7 @@
     <hyperlink r:id="rId861" ref="A426"/>
     <hyperlink r:id="rId862" ref="C426"/>
     <hyperlink r:id="rId863" ref="I426"/>
-    <hyperlink r:id="rId864" ref="A427"/>
+    <hyperlink r:id="rId864" location="leaderboard" ref="A427"/>
     <hyperlink r:id="rId865" ref="C427"/>
     <hyperlink r:id="rId866" ref="I427"/>
     <hyperlink r:id="rId867" ref="A428"/>

</xml_diff>

<commit_message>
refine the smell cases
</commit_message>
<xml_diff>
--- a/result/Foundation Model Leaderboards.xlsx
+++ b/result/Foundation Model Leaderboards.xlsx
@@ -22266,7 +22266,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="23" t="s">
         <v>1376</v>
       </c>
     </row>
@@ -23072,7 +23072,7 @@
     </row>
     <row r="7">
       <c r="E7" s="5"/>
-      <c r="G7" s="25" t="s">
+      <c r="G7" s="27" t="s">
         <v>1060</v>
       </c>
     </row>

</xml_diff>

<commit_message>
refine a lb smell cases
</commit_message>
<xml_diff>
--- a/result/Foundation Model Leaderboards.xlsx
+++ b/result/Foundation Model Leaderboards.xlsx
@@ -3683,7 +3683,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2710" uniqueCount="1379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2711" uniqueCount="1379">
   <si>
     <t>Name</t>
   </si>
@@ -10740,8 +10740,8 @@
         <v>11</v>
       </c>
       <c r="G90" s="2"/>
-      <c r="H90" s="2">
-        <v>4.0</v>
+      <c r="H90" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="I90" s="3" t="s">
         <v>176</v>

</xml_diff>

<commit_message>
refine smell case state
</commit_message>
<xml_diff>
--- a/result/Foundation Model Leaderboards.xlsx
+++ b/result/Foundation Model Leaderboards.xlsx
@@ -25,6 +25,12 @@
     <author/>
   </authors>
   <commentList>
+    <comment authorId="0" ref="A335">
+      <text>
+        <t xml:space="preserve">https://mmbench-video.github.io
+	-Jimmy Zhao</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="F357">
       <text>
         <t xml:space="preserve">https://github.com/salesforce/QAConv?tab=readme-ov-file#leaderboard
@@ -15812,7 +15818,7 @@
         <v>696</v>
       </c>
       <c r="B335" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C335" s="3" t="s">
         <v>697</v>

</xml_diff>

<commit_message>
udpate the smell case state
</commit_message>
<xml_diff>
--- a/result/Foundation Model Leaderboards.xlsx
+++ b/result/Foundation Model Leaderboards.xlsx
@@ -3689,7 +3689,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2711" uniqueCount="1379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2712" uniqueCount="1380">
   <si>
     <t>Name</t>
   </si>
@@ -8172,6 +8172,9 @@
   </si>
   <si>
     <t>https://huggingface.co/spaces/mesolitica/malaysian-stt-leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/MIMIC-CDM/leaderboard/discussions/1</t>
   </si>
   <si>
     <t>https://huggingface.co/spaces/mlfoundations/VisIT-Bench-Leaderboard/discussions/2</t>
@@ -22123,7 +22126,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="5" t="s">
-        <v>1357</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="2">
@@ -22133,7 +22136,7 @@
     </row>
     <row r="3">
       <c r="A3" s="29" t="s">
-        <v>1358</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="4">
@@ -22153,7 +22156,7 @@
     </row>
     <row r="7">
       <c r="A7" s="23" t="s">
-        <v>1359</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="8">
@@ -22173,22 +22176,22 @@
     </row>
     <row r="11">
       <c r="A11" s="36" t="s">
-        <v>1360</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="19" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="6" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="19" t="s">
-        <v>1363</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="15">
@@ -22202,43 +22205,43 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="27" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="21" t="s">
-        <v>1364</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="29" t="s">
-        <v>1365</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="19" t="s">
-        <v>1366</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="35" t="s">
-        <v>1367</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="24" t="s">
-        <v>1368</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="25" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="29" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="25">
@@ -22248,32 +22251,32 @@
     </row>
     <row r="26">
       <c r="A26" s="25" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="6" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="29" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="19" t="s">
-        <v>1374</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="23" t="s">
-        <v>1375</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="23" t="s">
-        <v>1376</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="32">
@@ -22283,12 +22286,12 @@
     </row>
     <row r="33">
       <c r="A33" s="27" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="3" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="35">
@@ -55161,7 +55164,7 @@
       <c r="D81" s="2"/>
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
-      <c r="G81" s="19" t="s">
+      <c r="G81" s="23" t="s">
         <v>1304</v>
       </c>
     </row>
@@ -55172,7 +55175,7 @@
       <c r="D82" s="2"/>
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
-      <c r="G82" s="21" t="s">
+      <c r="G82" s="19" t="s">
         <v>1305</v>
       </c>
     </row>
@@ -55183,7 +55186,7 @@
       <c r="D83" s="2"/>
       <c r="E83" s="2"/>
       <c r="F83" s="2"/>
-      <c r="G83" s="6" t="s">
+      <c r="G83" s="21" t="s">
         <v>1306</v>
       </c>
     </row>
@@ -55249,8 +55252,8 @@
       <c r="D89" s="5"/>
       <c r="E89" s="5"/>
       <c r="F89" s="5"/>
-      <c r="G89" s="19" t="s">
-        <v>634</v>
+      <c r="G89" s="6" t="s">
+        <v>1312</v>
       </c>
     </row>
     <row r="90">
@@ -55260,8 +55263,8 @@
       <c r="D90" s="5"/>
       <c r="E90" s="5"/>
       <c r="F90" s="5"/>
-      <c r="G90" s="23" t="s">
-        <v>556</v>
+      <c r="G90" s="19" t="s">
+        <v>634</v>
       </c>
     </row>
     <row r="91">
@@ -55271,8 +55274,8 @@
       <c r="D91" s="2"/>
       <c r="E91" s="2"/>
       <c r="F91" s="2"/>
-      <c r="G91" s="19" t="s">
-        <v>1312</v>
+      <c r="G91" s="23" t="s">
+        <v>556</v>
       </c>
     </row>
     <row r="92">
@@ -55305,7 +55308,7 @@
       <c r="E94" s="2"/>
       <c r="F94" s="2"/>
       <c r="G94" s="19" t="s">
-        <v>665</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="95">
@@ -55315,8 +55318,8 @@
       <c r="D95" s="2"/>
       <c r="E95" s="2"/>
       <c r="F95" s="2"/>
-      <c r="G95" s="6" t="s">
-        <v>1315</v>
+      <c r="G95" s="19" t="s">
+        <v>665</v>
       </c>
     </row>
     <row r="96">
@@ -55326,7 +55329,7 @@
       <c r="D96" s="2"/>
       <c r="E96" s="2"/>
       <c r="F96" s="2"/>
-      <c r="G96" s="3" t="s">
+      <c r="G96" s="6" t="s">
         <v>1316</v>
       </c>
     </row>
@@ -55337,7 +55340,7 @@
       <c r="D97" s="2"/>
       <c r="E97" s="2"/>
       <c r="F97" s="2"/>
-      <c r="G97" s="6" t="s">
+      <c r="G97" s="3" t="s">
         <v>1317</v>
       </c>
     </row>
@@ -55436,8 +55439,8 @@
       <c r="D106" s="2"/>
       <c r="E106" s="2"/>
       <c r="F106" s="2"/>
-      <c r="G106" s="19" t="s">
-        <v>156</v>
+      <c r="G106" s="6" t="s">
+        <v>1326</v>
       </c>
     </row>
     <row r="107">
@@ -55447,8 +55450,8 @@
       <c r="D107" s="2"/>
       <c r="E107" s="2"/>
       <c r="F107" s="2"/>
-      <c r="G107" s="6" t="s">
-        <v>1326</v>
+      <c r="G107" s="19" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="108">
@@ -55546,7 +55549,7 @@
       <c r="D116" s="2"/>
       <c r="E116" s="2"/>
       <c r="F116" s="2"/>
-      <c r="G116" s="23" t="s">
+      <c r="G116" s="6" t="s">
         <v>1335</v>
       </c>
     </row>
@@ -55557,7 +55560,7 @@
       <c r="D117" s="2"/>
       <c r="E117" s="2"/>
       <c r="F117" s="2"/>
-      <c r="G117" s="6" t="s">
+      <c r="G117" s="23" t="s">
         <v>1336</v>
       </c>
     </row>
@@ -55579,7 +55582,7 @@
       <c r="D119" s="2"/>
       <c r="E119" s="2"/>
       <c r="F119" s="2"/>
-      <c r="G119" s="23" t="s">
+      <c r="G119" s="6" t="s">
         <v>1338</v>
       </c>
     </row>
@@ -55590,7 +55593,7 @@
       <c r="D120" s="2"/>
       <c r="E120" s="2"/>
       <c r="F120" s="2"/>
-      <c r="G120" s="6" t="s">
+      <c r="G120" s="23" t="s">
         <v>1339</v>
       </c>
     </row>
@@ -55602,7 +55605,7 @@
       <c r="E121" s="2"/>
       <c r="F121" s="2"/>
       <c r="G121" s="6" t="s">
-        <v>719</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="122">
@@ -55612,8 +55615,8 @@
       <c r="D122" s="5"/>
       <c r="E122" s="5"/>
       <c r="F122" s="5"/>
-      <c r="G122" s="3" t="s">
-        <v>1340</v>
+      <c r="G122" s="6" t="s">
+        <v>719</v>
       </c>
     </row>
     <row r="123">
@@ -55623,7 +55626,7 @@
       <c r="D123" s="2"/>
       <c r="E123" s="2"/>
       <c r="F123" s="2"/>
-      <c r="G123" s="23" t="s">
+      <c r="G123" s="3" t="s">
         <v>1341</v>
       </c>
     </row>
@@ -55634,7 +55637,7 @@
       <c r="D124" s="5"/>
       <c r="E124" s="5"/>
       <c r="F124" s="5"/>
-      <c r="G124" s="6" t="s">
+      <c r="G124" s="23" t="s">
         <v>1342</v>
       </c>
     </row>
@@ -55678,8 +55681,8 @@
       <c r="D128" s="2"/>
       <c r="E128" s="2"/>
       <c r="F128" s="2"/>
-      <c r="G128" s="23" t="s">
-        <v>477</v>
+      <c r="G128" s="6" t="s">
+        <v>1346</v>
       </c>
     </row>
     <row r="129">
@@ -55689,8 +55692,8 @@
       <c r="D129" s="2"/>
       <c r="E129" s="2"/>
       <c r="F129" s="2"/>
-      <c r="G129" s="19" t="s">
-        <v>1346</v>
+      <c r="G129" s="23" t="s">
+        <v>477</v>
       </c>
     </row>
     <row r="130">
@@ -55700,7 +55703,7 @@
       <c r="D130" s="2"/>
       <c r="E130" s="2"/>
       <c r="F130" s="2"/>
-      <c r="G130" s="23" t="s">
+      <c r="G130" s="19" t="s">
         <v>1347</v>
       </c>
     </row>
@@ -55711,7 +55714,7 @@
       <c r="D131" s="2"/>
       <c r="E131" s="2"/>
       <c r="F131" s="2"/>
-      <c r="G131" s="19" t="s">
+      <c r="G131" s="23" t="s">
         <v>1348</v>
       </c>
     </row>
@@ -55722,8 +55725,8 @@
       <c r="D132" s="2"/>
       <c r="E132" s="2"/>
       <c r="F132" s="2"/>
-      <c r="G132" s="23" t="s">
-        <v>939</v>
+      <c r="G132" s="19" t="s">
+        <v>1349</v>
       </c>
     </row>
     <row r="133">
@@ -55733,8 +55736,8 @@
       <c r="D133" s="2"/>
       <c r="E133" s="2"/>
       <c r="F133" s="2"/>
-      <c r="G133" s="6" t="s">
-        <v>1349</v>
+      <c r="G133" s="23" t="s">
+        <v>939</v>
       </c>
     </row>
     <row r="134">
@@ -55775,13 +55778,18 @@
       </c>
     </row>
     <row r="139">
-      <c r="G139" s="25" t="s">
+      <c r="G139" s="6" t="s">
         <v>1355</v>
       </c>
     </row>
     <row r="140">
-      <c r="G140" s="6" t="s">
+      <c r="G140" s="25" t="s">
         <v>1356</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="G141" s="6" t="s">
+        <v>1357</v>
       </c>
     </row>
     <row r="142">
@@ -55939,7 +55947,8 @@
     <hyperlink r:id="rId142" ref="G138"/>
     <hyperlink r:id="rId143" ref="G139"/>
     <hyperlink r:id="rId144" ref="G140"/>
+    <hyperlink r:id="rId145" ref="G141"/>
   </hyperlinks>
-  <drawing r:id="rId145"/>
+  <drawing r:id="rId146"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update smell case state
</commit_message>
<xml_diff>
--- a/result/Foundation Model Leaderboards.xlsx
+++ b/result/Foundation Model Leaderboards.xlsx
@@ -25,6 +25,12 @@
     <author/>
   </authors>
   <commentList>
+    <comment authorId="0" ref="H201">
+      <text>
+        <t xml:space="preserve">https://labelbox.com/blog/labelbox-leaderboards-redefining-ai-evaluation-with-private-transparent-and-human-centric-assessments
+	-Jimmy Zhao</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="A335">
       <text>
         <t xml:space="preserve">https://mmbench-video.github.io
@@ -445,9 +451,6 @@
     <comment authorId="0" ref="A204">
       <text>
         <t xml:space="preserve">https://hkubs.hku.hk/aimodelrankings/en
-	-Jimmy Zhao
-----
-https://github.com/TongjiFinLab/CFBenchmark
 	-Jimmy Zhao</t>
       </text>
     </comment>
@@ -508,6 +511,9 @@
     <comment authorId="0" ref="A328">
       <text>
         <t xml:space="preserve">https://huggingface.co/spaces/opencompass/opencompass-llm-leaderboard
+	-Jimmy Zhao
+----
+https://github.com/web-arena-x/visualwebarena
 	-Jimmy Zhao</t>
       </text>
     </comment>
@@ -660,6 +666,9 @@
     <comment authorId="0" ref="A414">
       <text>
         <t xml:space="preserve">https://github.com/CLUEbenchmark/SuperCLUE-Safety?tab=readme-ov-file#%E6%A8%A1%E5%9E%8B%E4%B8%8E%E6%A6%9C%E5%8D%95
+	-Jimmy Zhao
+----
+https://github.com/EleutherAI/lm_perplexity
 	-Jimmy Zhao</t>
       </text>
     </comment>
@@ -840,6 +849,18 @@
     <comment authorId="0" ref="F305">
       <text>
         <t xml:space="preserve">https://github.com/Yuliang-Liu/MultimodalOCR?tab=readme-ov-file#ocrbench
+	-Jimmy Zhao
+----
+https://ogb-save.stanford.edu/leaderboard
+	-Jimmy Zhao
+----
+https://ogb-save.stanford.edu/leaderboard
+	-Jimmy Zhao
+----
+https://ogb-save.stanford.edu/leaderboard
+	-Jimmy Zhao
+----
+https://ogb-save.stanford.edu/leaderboard
 	-Jimmy Zhao</t>
       </text>
     </comment>
@@ -1291,7 +1312,7 @@
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="F285">
+    <comment authorId="0" ref="F284">
       <text>
         <t xml:space="preserve">https://leaderboard.carla.org/submit
 	-Jimmy Zhao</t>
@@ -2128,6 +2149,9 @@
     <comment authorId="0" ref="A236">
       <text>
         <t xml:space="preserve">https://github.com/longvideobench/LongVideoBench?tab=readme-ov-file#initial-leaderboard
+	-Jimmy Zhao
+----
+https://github.com/TIGER-AI-Lab/LongICLBench?tab=readme-ov-file#%EF%B8%8F-model-evaluation
 	-Jimmy Zhao</t>
       </text>
     </comment>
@@ -2318,18 +2342,6 @@
     <comment authorId="0" ref="F306">
       <text>
         <t xml:space="preserve">https://huggingface.co/spaces/valory/olas-prediction-leaderboard/discussions/3
-	-Jimmy Zhao
-----
-https://ogb-save.stanford.edu/leaderboard
-	-Jimmy Zhao
-----
-https://ogb-save.stanford.edu/leaderboard
-	-Jimmy Zhao
-----
-https://ogb-save.stanford.edu/leaderboard
-	-Jimmy Zhao
-----
-https://ogb-save.stanford.edu/leaderboard
 	-Jimmy Zhao</t>
       </text>
     </comment>
@@ -2399,12 +2411,6 @@
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A237">
-      <text>
-        <t xml:space="preserve">https://github.com/TIGER-AI-Lab/LongICLBench?tab=readme-ov-file#%EF%B8%8F-model-evaluation
-	-Jimmy Zhao</t>
-      </text>
-    </comment>
     <comment authorId="0" ref="A215">
       <text>
         <t xml:space="preserve">https://www.salesforceairesearch.com/crm-benchmark
@@ -2448,7 +2454,7 @@
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="H306">
+    <comment authorId="0" ref="H305">
       <text>
         <t xml:space="preserve">https://github.com/allenai/CommonGen-Eval?tab=readme-ov-file#run-gpt-4-based-evaluation
 	-Jimmy Zhao</t>
@@ -2466,7 +2472,7 @@
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I285">
+    <comment authorId="0" ref="I284">
       <text>
         <t xml:space="preserve">https://leaderboard.carla.org/about
 	-Jimmy Zhao</t>
@@ -2514,13 +2520,13 @@
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B306">
+    <comment authorId="0" ref="B305">
       <text>
         <t xml:space="preserve">https://github.com/allenai/CommonGen-Eval
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B399">
+    <comment authorId="0" ref="B398">
       <text>
         <t xml:space="preserve">https://github.com/MAGIC-AI4Med/MMedLM
 	-Jimmy Zhao</t>
@@ -2532,7 +2538,7 @@
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B284">
+    <comment authorId="0" ref="B283">
       <text>
         <t xml:space="preserve">https://github.com/YihongDong/CDD-TED4LLMs
 	-Jimmy Zhao</t>
@@ -2544,7 +2550,7 @@
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B300">
+    <comment authorId="0" ref="B299">
       <text>
         <t xml:space="preserve">https://github.com/mesolitica/malaysian-stt-benchmarks
 	-Jimmy Zhao
@@ -2643,19 +2649,19 @@
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I399">
+    <comment authorId="0" ref="I398">
       <text>
         <t xml:space="preserve">https://medium.com/@tao.yu/spider-one-more-step-towards-natural-language-interfaces-to-databases-62298dc6df3c
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I463">
+    <comment authorId="0" ref="I462">
       <text>
         <t xml:space="preserve">https://huggingface.co/blog/manu/colpali
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I329">
+    <comment authorId="0" ref="I328">
       <text>
         <t xml:space="preserve">https://arxiv.org/pdf/2406.07545
 	-Jimmy Zhao</t>
@@ -2685,7 +2691,7 @@
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I364">
+    <comment authorId="0" ref="I363">
       <text>
         <t xml:space="preserve">https://arxiv.org/html/2406.12066v2
 	-Jimmy Zhao</t>
@@ -2717,13 +2723,13 @@
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I443">
+    <comment authorId="0" ref="I442">
       <text>
         <t xml:space="preserve">https://llm.extractum.io/static/blog/?id=ugi-leaderboard
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I438">
+    <comment authorId="0" ref="I437">
       <text>
         <t xml:space="preserve">https://www.trustbit.tech/en/llm-leaderboard-mai-2024
 	-Jimmy Zhao</t>
@@ -2735,7 +2741,7 @@
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I256">
+    <comment authorId="0" ref="I255">
       <text>
         <t xml:space="preserve">https://www.philschmid.de/evaluate-llm-mixeval
 	-Jimmy Zhao</t>
@@ -2759,7 +2765,7 @@
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I341">
+    <comment authorId="0" ref="I340">
       <text>
         <t xml:space="preserve">https://arxiv.org/html/2405.00732v1
 	-Jimmy Zhao</t>
@@ -2777,7 +2783,7 @@
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I303">
+    <comment authorId="0" ref="I302">
       <text>
         <t xml:space="preserve">https://arxiv.org/html/2406.06462v2
 	-Jimmy Zhao
@@ -2830,7 +2836,7 @@
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I290">
+    <comment authorId="0" ref="I289">
       <text>
         <t xml:space="preserve">https://arxiv.org/html/2405.04520v1
 	-Jimmy Zhao</t>
@@ -2852,7 +2858,7 @@
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I270">
+    <comment authorId="0" ref="I269">
       <text>
         <t xml:space="preserve">https://arxiv.org/html/2312.14852v3
 	-Jimmy Zhao</t>
@@ -2876,7 +2882,7 @@
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I260">
+    <comment authorId="0" ref="I259">
       <text>
         <t xml:space="preserve">https://arxiv.org/pdf/2406.04264
 	-Jimmy Zhao
@@ -2891,55 +2897,55 @@
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I459">
+    <comment authorId="0" ref="I458">
       <text>
         <t xml:space="preserve">https://arxiv.org/pdf/2406.09367
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I421">
+    <comment authorId="0" ref="I420">
       <text>
         <t xml:space="preserve">https://mp.weixin.qq.com/s/pNLlWesPOIeCfHu5xVfOGg
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I422">
+    <comment authorId="0" ref="I421">
       <text>
         <t xml:space="preserve">https://mp.weixin.qq.com/s/dUfF2TfYKrR3ZTn-nhpH-w
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I413">
+    <comment authorId="0" ref="I412">
       <text>
         <t xml:space="preserve">https://mp.weixin.qq.com/s/eIS7BjFYmyby2gpSd875Hw
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I411">
+    <comment authorId="0" ref="I410">
       <text>
         <t xml:space="preserve">https://mp.weixin.qq.com/s/QPeUu5ThP2f0dKEPDuFqxA
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I410">
+    <comment authorId="0" ref="I409">
       <text>
         <t xml:space="preserve">https://mp.weixin.qq.com/s/emW_g5A8DKTFojvWFnsrqQ
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="H415">
+    <comment authorId="0" ref="H414">
       <text>
         <t xml:space="preserve">https://github.com/EleutherAI/lm_perplexity/issues/2
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="H223">
+    <comment authorId="0" ref="H222">
       <text>
         <t xml:space="preserve">https://matheval.ai/evaluation
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I223">
+    <comment authorId="0" ref="I222">
       <text>
         <t xml:space="preserve">https://ai.100tal.com
 	-Jimmy Zhao
@@ -2950,13 +2956,13 @@
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B223">
+    <comment authorId="0" ref="B222">
       <text>
         <t xml:space="preserve">https://github.com/math-eval/MathEval
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B248">
+    <comment authorId="0" ref="B247">
       <text>
         <t xml:space="preserve">https://github.com/THUNLP-MT/StableToolBench
 	-Jimmy Zhao</t>
@@ -2968,7 +2974,7 @@
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I445">
+    <comment authorId="0" ref="I444">
       <text>
         <t xml:space="preserve">https://arxiv.org/pdf/2403.20331
 	-Jimmy Zhao</t>
@@ -2989,7 +2995,7 @@
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I392">
+    <comment authorId="0" ref="I391">
       <text>
         <t xml:space="preserve">https://scale.com/
 	-Jimmy Zhao</t>
@@ -3007,7 +3013,7 @@
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I219">
+    <comment authorId="0" ref="I218">
       <text>
         <t xml:space="preserve">https://github.com/evalplus/repoqa
 	-Jimmy Zhao
@@ -3016,13 +3022,13 @@
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I242">
+    <comment authorId="0" ref="I241">
       <text>
         <t xml:space="preserve">https://arxiv.org/pdf/2405.12209
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I455">
+    <comment authorId="0" ref="I454">
       <text>
         <t xml:space="preserve">https://www.reka.ai/news/vibe-eval
 	-Jimmy Zhao
@@ -3030,19 +3036,19 @@
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I417">
+    <comment authorId="0" ref="I416">
       <text>
         <t xml:space="preserve">https://www.cluebenchmarks.com/superclue_role.html
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I416">
+    <comment authorId="0" ref="I415">
       <text>
         <t xml:space="preserve">https://www.cluebenchmarks.com/superclue_rag.html
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I203">
+    <comment authorId="0" ref="I202">
       <text>
         <t xml:space="preserve">https://ai.meta.com/blog/openeqa-embodied-question-answering-robotics-ar-glasses/
 	-Jimmy Zhao</t>
@@ -3054,18 +3060,24 @@
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I273">
+    <comment authorId="0" ref="I272">
       <text>
         <t xml:space="preserve">Algorithm: Length Penalty
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I204">
+    <comment authorId="0" ref="I203">
       <text>
         <t xml:space="preserve">https://github.com/open-compass/opencompass/blob/main/configs/datasets/OpenFinData/OpenFinData.md
 	-Jimmy Zhao
 ----
 due to benchmark evolution
+	-Jimmy Zhao</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A203">
+      <text>
+        <t xml:space="preserve">https://github.com/TongjiFinLab/CFBenchmark
 	-Jimmy Zhao</t>
       </text>
     </comment>
@@ -3081,13 +3093,13 @@
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="H209">
+    <comment authorId="0" ref="H208">
       <text>
         <t xml:space="preserve">https://github.com/NousResearch/finetuning-subnet/blob/master/docs/validator.md
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A209">
+    <comment authorId="0" ref="A208">
       <text>
         <t xml:space="preserve">model- and data-centric leaderboards
 	-Jimmy Zhao
@@ -3098,67 +3110,67 @@
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I238">
+    <comment authorId="0" ref="I237">
       <text>
         <t xml:space="preserve">https://toloka.ai/talk-to-us/
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I415">
+    <comment authorId="0" ref="I414">
       <text>
         <t xml:space="preserve">https://www.cluebenchmarks.com/superclue_open.html
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I412">
+    <comment authorId="0" ref="I411">
       <text>
         <t xml:space="preserve">https://www.cluebenchmarks.com/superclue_industry.html
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I405">
+    <comment authorId="0" ref="I404">
       <text>
         <t xml:space="preserve">https://www.cluebenchmarks.com/superclue.html
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I407">
+    <comment authorId="0" ref="I406">
       <text>
         <t xml:space="preserve">https://www.cluebenchmarks.com/superclue_agent.html
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I408">
+    <comment authorId="0" ref="I407">
       <text>
         <t xml:space="preserve">https://www.cluebenchmarks.com/superclue_auto.html
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I409">
+    <comment authorId="0" ref="I408">
       <text>
         <t xml:space="preserve">https://www.cluebenchmarks.com/superclue_code3.html
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I414">
+    <comment authorId="0" ref="I413">
       <text>
         <t xml:space="preserve">https://www.cluebenchmarks.com/superclue_math6.html
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I418">
+    <comment authorId="0" ref="I417">
       <text>
         <t xml:space="preserve">https://www.cluebenchmarks.com/superclue_safety.html
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I291">
+    <comment authorId="0" ref="I290">
       <text>
         <t xml:space="preserve">https://nexusflow.ai/blogs/ravenv2
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I268">
+    <comment authorId="0" ref="I267">
       <text>
         <t xml:space="preserve">https://coreymorrisdata.medium.com/preliminary-analysis-of-mmlu-evaluation-data-insights-from-500-open-source-models-e67885aa364b
 	-Jimmy Zhao
@@ -3211,23 +3223,6 @@
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A329">
-      <text>
-        <t xml:space="preserve">https://github.com/web-arena-x/visualwebarena
-	-Jimmy Zhao
-----
-https://huggingface.co/spaces/opencompass/open_vlm_leaderboard
-	-Jimmy Zhao
-https://openxlab.org.cn/apps/detail/kennyutc/open_mllm_leaderboard
-	-Jimmy Zhao</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="A415">
-      <text>
-        <t xml:space="preserve">https://github.com/EleutherAI/lm_perplexity
-	-Jimmy Zhao</t>
-      </text>
-    </comment>
     <comment authorId="0" ref="B163">
       <text>
         <t xml:space="preserve">https://github.com/tsb0601/MMVP
@@ -3240,7 +3235,7 @@
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B250">
+    <comment authorId="0" ref="B249">
       <text>
         <t xml:space="preserve">https://github.com/salesforce/factualNLG
 	-Jimmy Zhao</t>
@@ -3330,19 +3325,19 @@
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I249">
+    <comment authorId="0" ref="I248">
       <text>
         <t xml:space="preserve">https://whoops-benchmark.github.io/
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I262">
+    <comment authorId="0" ref="I261">
       <text>
         <t xml:space="preserve">https://huggingface.co/spaces/mlfoundations/VisIT-Bench-Leaderboard/discussions/1
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I272">
+    <comment authorId="0" ref="I271">
       <text>
         <t xml:space="preserve">https://huggingface.co/spaces/nlphuji/WHOOPS-Leaderboard-Full/discussions/1
 	-Jimmy Zhao</t>
@@ -3354,7 +3349,7 @@
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I209">
+    <comment authorId="0" ref="I208">
       <text>
         <t xml:space="preserve">https://github.com/NousResearch/finetuning-subnet/blob/master/docs/validator.md#getting-started
 	-Jimmy Zhao
@@ -3368,7 +3363,7 @@
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B209">
+    <comment authorId="0" ref="B208">
       <text>
         <t xml:space="preserve">https://github.com/NousResearch/finetuning-subnet
 	-Jimmy Zhao
@@ -3419,7 +3414,7 @@
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I248">
+    <comment authorId="0" ref="I247">
       <text>
         <t xml:space="preserve">https://github.com/sylinrl/TruthfulQA/issues/8
 	-Jimmy Zhao</t>
@@ -3470,7 +3465,7 @@
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I250">
+    <comment authorId="0" ref="I249">
       <text>
         <t xml:space="preserve">IEEE International Conference on Acoustics, Speech and Signal Processing
 	-Jimmy Zhao</t>
@@ -3505,6 +3500,14 @@
     <comment authorId="0" ref="I69">
       <text>
         <t xml:space="preserve">https://github.com/EQ-bench/EQ-Bench
+	-Jimmy Zhao</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A329">
+      <text>
+        <t xml:space="preserve">https://huggingface.co/spaces/opencompass/open_vlm_leaderboard
+	-Jimmy Zhao
+https://openxlab.org.cn/apps/detail/kennyutc/open_mllm_leaderboard
 	-Jimmy Zhao</t>
       </text>
     </comment>
@@ -3595,7 +3598,7 @@
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A269">
+    <comment authorId="0" ref="A268">
       <text>
         <t xml:space="preserve">https://github.com/tjunlp-lab/Awesome-LLMs-Evaluation-Papers/issues/24
 	-Jimmy Zhao</t>
@@ -3645,7 +3648,7 @@
 	-Jimmy Zhao</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B373">
+    <comment authorId="0" ref="B372">
       <text>
         <t xml:space="preserve">https://huggingface.co/spaces/nlphuji/WHOOPS-Leaderboard
 	-Jimmy Zhao
@@ -3689,7 +3692,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2726" uniqueCount="1385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2727" uniqueCount="1385">
   <si>
     <t>Name</t>
   </si>
@@ -14735,6 +14738,23 @@
       <c r="I221" s="23" t="s">
         <v>446</v>
       </c>
+      <c r="J221" s="26"/>
+      <c r="K221" s="26"/>
+      <c r="L221" s="26"/>
+      <c r="M221" s="26"/>
+      <c r="N221" s="26"/>
+      <c r="O221" s="26"/>
+      <c r="P221" s="26"/>
+      <c r="Q221" s="26"/>
+      <c r="R221" s="26"/>
+      <c r="S221" s="26"/>
+      <c r="T221" s="26"/>
+      <c r="U221" s="26"/>
+      <c r="V221" s="26"/>
+      <c r="W221" s="26"/>
+      <c r="X221" s="26"/>
+      <c r="Y221" s="26"/>
+      <c r="Z221" s="26"/>
     </row>
     <row r="222">
       <c r="A222" s="4" t="s">
@@ -14756,23 +14776,6 @@
       <c r="I222" s="43" t="s">
         <v>448</v>
       </c>
-      <c r="J222" s="26"/>
-      <c r="K222" s="26"/>
-      <c r="L222" s="26"/>
-      <c r="M222" s="26"/>
-      <c r="N222" s="26"/>
-      <c r="O222" s="26"/>
-      <c r="P222" s="26"/>
-      <c r="Q222" s="26"/>
-      <c r="R222" s="26"/>
-      <c r="S222" s="26"/>
-      <c r="T222" s="26"/>
-      <c r="U222" s="26"/>
-      <c r="V222" s="26"/>
-      <c r="W222" s="26"/>
-      <c r="X222" s="26"/>
-      <c r="Y222" s="26"/>
-      <c r="Z222" s="26"/>
     </row>
     <row r="223">
       <c r="A223" s="8" t="s">
@@ -15581,6 +15584,23 @@
       <c r="H261" s="9" t="s">
         <v>81</v>
       </c>
+      <c r="J261" s="26"/>
+      <c r="K261" s="26"/>
+      <c r="L261" s="26"/>
+      <c r="M261" s="26"/>
+      <c r="N261" s="26"/>
+      <c r="O261" s="26"/>
+      <c r="P261" s="26"/>
+      <c r="Q261" s="26"/>
+      <c r="R261" s="26"/>
+      <c r="S261" s="26"/>
+      <c r="T261" s="26"/>
+      <c r="U261" s="26"/>
+      <c r="V261" s="26"/>
+      <c r="W261" s="26"/>
+      <c r="X261" s="26"/>
+      <c r="Y261" s="26"/>
+      <c r="Z261" s="26"/>
     </row>
     <row r="262">
       <c r="A262" s="4" t="s">
@@ -15604,23 +15624,6 @@
         <v>32</v>
       </c>
       <c r="I262" s="44"/>
-      <c r="J262" s="26"/>
-      <c r="K262" s="26"/>
-      <c r="L262" s="26"/>
-      <c r="M262" s="26"/>
-      <c r="N262" s="26"/>
-      <c r="O262" s="26"/>
-      <c r="P262" s="26"/>
-      <c r="Q262" s="26"/>
-      <c r="R262" s="26"/>
-      <c r="S262" s="26"/>
-      <c r="T262" s="26"/>
-      <c r="U262" s="26"/>
-      <c r="V262" s="26"/>
-      <c r="W262" s="26"/>
-      <c r="X262" s="26"/>
-      <c r="Y262" s="26"/>
-      <c r="Z262" s="26"/>
     </row>
     <row r="263">
       <c r="A263" s="8" t="s">
@@ -15725,6 +15728,23 @@
       <c r="I267" s="35" t="s">
         <v>551</v>
       </c>
+      <c r="J267" s="26"/>
+      <c r="K267" s="26"/>
+      <c r="L267" s="26"/>
+      <c r="M267" s="26"/>
+      <c r="N267" s="26"/>
+      <c r="O267" s="26"/>
+      <c r="P267" s="26"/>
+      <c r="Q267" s="26"/>
+      <c r="R267" s="26"/>
+      <c r="S267" s="26"/>
+      <c r="T267" s="26"/>
+      <c r="U267" s="26"/>
+      <c r="V267" s="26"/>
+      <c r="W267" s="26"/>
+      <c r="X267" s="26"/>
+      <c r="Y267" s="26"/>
+      <c r="Z267" s="26"/>
     </row>
     <row r="268">
       <c r="A268" s="4" t="s">
@@ -15743,23 +15763,6 @@
         <v>4.0</v>
       </c>
       <c r="I268" s="44"/>
-      <c r="J268" s="26"/>
-      <c r="K268" s="26"/>
-      <c r="L268" s="26"/>
-      <c r="M268" s="26"/>
-      <c r="N268" s="26"/>
-      <c r="O268" s="26"/>
-      <c r="P268" s="26"/>
-      <c r="Q268" s="26"/>
-      <c r="R268" s="26"/>
-      <c r="S268" s="26"/>
-      <c r="T268" s="26"/>
-      <c r="U268" s="26"/>
-      <c r="V268" s="26"/>
-      <c r="W268" s="26"/>
-      <c r="X268" s="26"/>
-      <c r="Y268" s="26"/>
-      <c r="Z268" s="26"/>
     </row>
     <row r="269">
       <c r="A269" s="8" t="s">
@@ -16198,6 +16201,23 @@
       <c r="I289" s="23" t="s">
         <v>600</v>
       </c>
+      <c r="J289" s="26"/>
+      <c r="K289" s="26"/>
+      <c r="L289" s="26"/>
+      <c r="M289" s="26"/>
+      <c r="N289" s="26"/>
+      <c r="O289" s="26"/>
+      <c r="P289" s="26"/>
+      <c r="Q289" s="26"/>
+      <c r="R289" s="26"/>
+      <c r="S289" s="26"/>
+      <c r="T289" s="26"/>
+      <c r="U289" s="26"/>
+      <c r="V289" s="26"/>
+      <c r="W289" s="26"/>
+      <c r="X289" s="26"/>
+      <c r="Y289" s="26"/>
+      <c r="Z289" s="26"/>
     </row>
     <row r="290">
       <c r="A290" s="19" t="s">
@@ -16221,23 +16241,6 @@
       <c r="I290" s="43" t="s">
         <v>604</v>
       </c>
-      <c r="J290" s="26"/>
-      <c r="K290" s="26"/>
-      <c r="L290" s="26"/>
-      <c r="M290" s="26"/>
-      <c r="N290" s="26"/>
-      <c r="O290" s="26"/>
-      <c r="P290" s="26"/>
-      <c r="Q290" s="26"/>
-      <c r="R290" s="26"/>
-      <c r="S290" s="26"/>
-      <c r="T290" s="26"/>
-      <c r="U290" s="26"/>
-      <c r="V290" s="26"/>
-      <c r="W290" s="26"/>
-      <c r="X290" s="26"/>
-      <c r="Y290" s="26"/>
-      <c r="Z290" s="26"/>
     </row>
     <row r="291">
       <c r="A291" s="8" t="s">
@@ -18282,8 +18285,8 @@
         <v>11</v>
       </c>
       <c r="G390" s="7"/>
-      <c r="H390" s="5">
-        <v>4.0</v>
+      <c r="H390" s="5" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="391">
@@ -18788,6 +18791,23 @@
       <c r="H415" s="9">
         <v>4.0</v>
       </c>
+      <c r="J415" s="26"/>
+      <c r="K415" s="26"/>
+      <c r="L415" s="26"/>
+      <c r="M415" s="26"/>
+      <c r="N415" s="26"/>
+      <c r="O415" s="26"/>
+      <c r="P415" s="26"/>
+      <c r="Q415" s="26"/>
+      <c r="R415" s="26"/>
+      <c r="S415" s="26"/>
+      <c r="T415" s="26"/>
+      <c r="U415" s="26"/>
+      <c r="V415" s="26"/>
+      <c r="W415" s="26"/>
+      <c r="X415" s="26"/>
+      <c r="Y415" s="26"/>
+      <c r="Z415" s="26"/>
     </row>
     <row r="416">
       <c r="A416" s="4" t="s">
@@ -18884,23 +18904,6 @@
       <c r="I418" s="43" t="s">
         <v>877</v>
       </c>
-      <c r="J418" s="26"/>
-      <c r="K418" s="26"/>
-      <c r="L418" s="26"/>
-      <c r="M418" s="26"/>
-      <c r="N418" s="26"/>
-      <c r="O418" s="26"/>
-      <c r="P418" s="26"/>
-      <c r="Q418" s="26"/>
-      <c r="R418" s="26"/>
-      <c r="S418" s="26"/>
-      <c r="T418" s="26"/>
-      <c r="U418" s="26"/>
-      <c r="V418" s="26"/>
-      <c r="W418" s="26"/>
-      <c r="X418" s="26"/>
-      <c r="Y418" s="26"/>
-      <c r="Z418" s="26"/>
     </row>
     <row r="419">
       <c r="A419" s="8" t="s">
@@ -19035,6 +19038,23 @@
       <c r="I424" s="24" t="s">
         <v>893</v>
       </c>
+      <c r="J424" s="26"/>
+      <c r="K424" s="26"/>
+      <c r="L424" s="26"/>
+      <c r="M424" s="26"/>
+      <c r="N424" s="26"/>
+      <c r="O424" s="26"/>
+      <c r="P424" s="26"/>
+      <c r="Q424" s="26"/>
+      <c r="R424" s="26"/>
+      <c r="S424" s="26"/>
+      <c r="T424" s="26"/>
+      <c r="U424" s="26"/>
+      <c r="V424" s="26"/>
+      <c r="W424" s="26"/>
+      <c r="X424" s="26"/>
+      <c r="Y424" s="26"/>
+      <c r="Z424" s="26"/>
     </row>
     <row r="425">
       <c r="A425" s="8" t="s">
@@ -19058,23 +19078,6 @@
         <v>32</v>
       </c>
       <c r="I425" s="25"/>
-      <c r="J425" s="26"/>
-      <c r="K425" s="26"/>
-      <c r="L425" s="26"/>
-      <c r="M425" s="26"/>
-      <c r="N425" s="26"/>
-      <c r="O425" s="26"/>
-      <c r="P425" s="26"/>
-      <c r="Q425" s="26"/>
-      <c r="R425" s="26"/>
-      <c r="S425" s="26"/>
-      <c r="T425" s="26"/>
-      <c r="U425" s="26"/>
-      <c r="V425" s="26"/>
-      <c r="W425" s="26"/>
-      <c r="X425" s="26"/>
-      <c r="Y425" s="26"/>
-      <c r="Z425" s="26"/>
     </row>
     <row r="426">
       <c r="A426" s="4" t="s">
@@ -22460,22 +22463,15 @@
       <c r="F809" s="61"/>
       <c r="H809" s="61"/>
     </row>
-    <row r="810">
-      <c r="B810" s="61"/>
-      <c r="D810" s="61"/>
-      <c r="E810" s="61"/>
-      <c r="F810" s="61"/>
-      <c r="H810" s="61"/>
-    </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B2:B810">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B2:B809">
       <formula1>"gh,gh,hf,gh,hf,ip,gh,ip,gh,pwc,hf,hf,ip,ip,Host platforms,pwc,ss,ip,ss,gh,ss"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:F482">
       <formula1>"Has any submission channel/protocol?,y"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D810">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D809">
       <formula1>"Has many major releases?,y"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H2:H482">
@@ -22487,13 +22483,13 @@
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E482">
       <formula1>"Attaches model provenance?,y"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H2:H810">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H2:H809">
       <formula1>"1,1,4,1,4,5,2,2,4,3,4,4,5,5,Workflow patterns,1,5,1,2,4"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:F810">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:F809">
       <formula1>"Has any submission channel/protocol?,y"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E810">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E809">
       <formula1>"Attaches model provenance?,y"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
update smell case report
</commit_message>
<xml_diff>
--- a/result/Foundation Model Leaderboards.xlsx
+++ b/result/Foundation Model Leaderboards.xlsx
@@ -7440,969 +7440,969 @@
     <t>https://github.com/OpenGVLab/Multi-Modality-Arena/issues/19</t>
   </si>
   <si>
+    <t>https://github.com/thu-coai/Safety-Prompts/issues/23</t>
+  </si>
+  <si>
+    <t>https://github.com/whoops-benchmark/whoops-benchmark.github.io/issues/1</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/25</t>
+  </si>
+  <si>
+    <t>https://github.com/stanford-crfm/helm/issues/2205</t>
+  </si>
+  <si>
+    <t>https://github.com/CLUEbenchmark/SuperCLUE/issues/41</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/26</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/mlabonne/Yet_Another_LLM_Leaderboard/discussions/8</t>
+  </si>
+  <si>
+    <t>https://github.com/Q-Future/Q-Bench/issues/11</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/27</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/bhaskartripathi/llm_leaderboards360/discussions/2</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/28</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/29</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/onekq-ai/WebApp1K-models-leaderboard/discussions/2</t>
+  </si>
+  <si>
+    <t>https://github.com/stanford-crfm/helm/issues/2034</t>
+  </si>
+  <si>
+    <t>https://github.com/LudwigStumpp/llm-leaderboard/issues/9</t>
+  </si>
+  <si>
+    <t>https://github.com/embeddings-benchmark/mteb/issues/191</t>
+  </si>
+  <si>
+    <t>https://github.com/LudwigStumpp/llm-leaderboard/issues/10</t>
+  </si>
+  <si>
+    <t>https://github.com/flageval-baai/FlagEval/issues/34</t>
+  </si>
+  <si>
+    <t>https://github.com/stanford-crfm/helm/issues/2060</t>
+  </si>
+  <si>
+    <t>https://github.com/OpenGVLab/Multi-Modality-Arena/issues/25</t>
+  </si>
+  <si>
+    <t>https://github.com/flageval-baai/FlagEval/issues/35</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/32</t>
+  </si>
+  <si>
+    <t>https://github.com/THU-KEG/KoLA/issues/8</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/38</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/20221205184917/https://paperswithcode.com/sota/image-classification-on-humaneval</t>
+  </si>
+  <si>
+    <t>https://github.com/Q-Future/Chinese-Q-Bench/issues/2</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/20240222011501/https://paperswithcode.com/sota/text-generation-on-humaneval</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/mlabonne/Yet_Another_LLM_Leaderboard/discussions/11</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/speakleash/open_pl_llm_leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://github.com/stanford-crfm/helm/issues/2062</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/41</t>
+  </si>
+  <si>
+    <t>https://github.com/THU-KEG/KoLA/issues/6</t>
+  </si>
+  <si>
+    <t>https://github.com/stanford-crfm/helm/issues/2351</t>
+  </si>
+  <si>
+    <t>https://github.com/stanford-crfm/helm/issues/2239</t>
+  </si>
+  <si>
+    <t>https://github.com/stanford-crfm/helm/issues/2176</t>
+  </si>
+  <si>
+    <t>https://github.com/THU-KEG/KoLA/issues/7</t>
+  </si>
+  <si>
+    <t>https://github.com/THU-KEG/KoLA/issues/2</t>
+  </si>
+  <si>
+    <t>https://github.com/THU-KEG/KoLA/issues/5</t>
+  </si>
+  <si>
+    <t>https://github.com/CLUEbenchmark/SuperCLUE-Code3/issues/2</t>
+  </si>
+  <si>
+    <t>https://github.com/open-compass/LawBench/issues/7</t>
+  </si>
+  <si>
+    <t>https://github.com/msamwelmollel/Swahili_LLM_Leaderboard/issues/2</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/upstage/open-ko-llm-leaderboard/discussions/28</t>
+  </si>
+  <si>
+    <t>https://github.com/jeinlee1991/chinese-llm-benchmark/issues/19</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/30</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/100</t>
+  </si>
+  <si>
+    <t>https://github.com/open-compass/opencompass/discussions/784</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/31</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/101</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/opencompass/open_vlm_leaderboard/discussions/3</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/33</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/102</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/opencompass/open_vlm_leaderboard/discussions/4</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/34</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/103</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/opencompass/open_vlm_leaderboard/discussions/5</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/35</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/104</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/TwinDoc/leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/36</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/105</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/37</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/106</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/mii-llm/open_ita_llm_leaderboard/discussions/4</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/40</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/107</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/valory/olas-prediction-leaderboard/discussions/3</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/42</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/108</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/43</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/109</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/44</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/110</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/45</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/111</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/46</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/112</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/47</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/113</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/48</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/114</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/49</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/115</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/50</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/116</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/52</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/117</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/53</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/118</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/54</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/119</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/55</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/120</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/56</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/121</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/57</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/122</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/58</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/123</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/59</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/124</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/60</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/125</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/61</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/126</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/62</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/127</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/63</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/128</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/64</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/129</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/65</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/130</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/66</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/131</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/67</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/132</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/68</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/133</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/69</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/134</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/70</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/135</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/71</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/136</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/72</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/137</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/73</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/138</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/74</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/139</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/75</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/140</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/76</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/141</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/77</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/142</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/78</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/143</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/79</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/144</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/80</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/149</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/81</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/145</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/82</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/146</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/83</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/147</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/84</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/148</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/150</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/151</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/152</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/153</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/154</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/155</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/156</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/157</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/158</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/159</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/160</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/161</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/162</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/163</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/164</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/85</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/86</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/87</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/88</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/89</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/90</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/91</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/92</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/93</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/94</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/95</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/96</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/97</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/98</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/99</t>
+  </si>
+  <si>
+    <t>https://github.com/stanford-crfm/helm/issues/2008</t>
+  </si>
+  <si>
+    <t>https://github.com/stanford-crfm/helm/issues/2010</t>
+  </si>
+  <si>
+    <t>https://github.com/THU-KEG/KoLA/issues/18</t>
+  </si>
+  <si>
+    <t>https://github.com/tjunlp-lab/Awesome-LLMs-Evaluation-Papers/issues/27</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/instructkr/ko-chatbot-arena-leaderboard/discussions/4</t>
+  </si>
+  <si>
+    <t>https://github.com/OpenGVLab/Multi-Modality-Arena/issues/26</t>
+  </si>
+  <si>
+    <t>https://github.com/THU-KEG/KoLA/issues/17</t>
+  </si>
+  <si>
+    <t>https://github.com/flageval-baai/FlagEval/issues/36</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/archit11/Hindi_LLM_arena/discussions/1</t>
+  </si>
+  <si>
+    <t>https://github.com/paperswithcode/sota-extractor/issues/39</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/cambioml/parser-leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://github.com/stanford-crfm/helm/issues/2039</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/instructkr/ko-chatbot-arena-leaderboard/discussions/5</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/0x1668/open_llm_leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/NexaAIDev/domain_llm_leaderboard/discussions/4</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/0x9/finetuning_subnet_leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/0x9/pretraining-leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/Aarifkhan/leaderboard-results-to-modelcard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/abidlabs/chatbot-arena-leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/abidlabs/mteb-leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/AI-Vietnam/prompt-translation-vie-leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/aichampions/open_llm_leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/Alfasign/open_llm_leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/anglesplato/Deep-Reinforcement-Learning-Leaderboard-V2/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/anirudh937/open_llm_leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/arshy/leaderboard-docker/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/arshy/leaderboard-gradio/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/arshy/leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/asir0z/open_llm_leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/autogenCTF/agent_ctf_leaderboard/discussions/3</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/automerger/Yet_Another_LLM_Leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/awacke1/CanAICode-Leaderboard-Customized/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/b1sheng/kg_llm_leaderboard_test/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/BioMed-VITAL/leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/bittensor-dataset/leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/CathieDaDa/LLM_leaderboard/discussions/3</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/CDT-BMAI-GP/biomed_probing_leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/choco9966/open-ko-llm-leaderboard-old/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/Classroom-workshop/assignments-leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/crynux-ai/genki-dama-leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/CVPR/Leaderboard/discussions/2</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/DeepBrainz/open_llm_leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/deepcode-ai/deepcode-models-leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/demo-crafters/leaderboard/discussions/2</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/demo-leaderboard-backend/leaderboard/discussions/6</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/deprem-ml/intent-leaderboard-v13/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/deprem-ml/intent-leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/dimbyTa/open-llm-leaderboard-viz/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/Docfile/open_llm_leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/DontPlanToEnd/UGI-Leaderboard/discussions/4</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/ECCV2022/Leaderboard/discussions/2</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/esb/leaderboard/discussions/3</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/EuroPython2022/Leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/EuroSciPy2022/Leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/felixz/open_llm_leaderboard/discussions/2</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/freddyaboulton/gradio_leaderboard_demo/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/gblazex/leaderboard/discussions/5</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/gsaivinay/open_llm_leaderboard/discussions/4</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/gsaivinay/open_llm_leaderboard/discussions/5</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/hjzhou/chatbot-arena-leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/homunculus/Deep-Reinforcement-Learning-Leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/hubistrauss/princeton_benchmarks_leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/HuggingFaceH4/human_eval_llm_leaderboard/discussions/4</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/hugginglearners/Hearts_Leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/ICML2022/Leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/Infin/sn32-testnet-leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/JarvisKi/Stable_Tool_Bench_Leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/junior-labs/llm-colosseum/discussions/2</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/k8si/mteb_leaderboard_mtr/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/kbmlcoding/open_llm_leaderboard_free/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/kevinwang676/ocrbench-leaderboard/discussions/2</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/khhuiyh/AutoEval-Video_LeaderBoard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/Koshti10/leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/ludwigstumpp/llm-leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/macrocosm-os/finetuning-leaderboard/discussions/3</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/macrocosm-os/pretraining-leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/Manavshah/dippy-leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/mesolitica/malaysian-stt-leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/MIMIC-CDM/leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/mlfoundations/VisIT-Bench-Leaderboard/discussions/2</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/MohamedRashad/timm-leaderboard/discussions/2</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/Mollel/swahili-llm-leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/NAACL2022/Spaces-Leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/nan/leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/neelalex/leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/nlphuji/WHOOPS-Leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/nouamanetazi/mteb-leaderboard-old/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/Nymbo/leaderboard_main/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/opencompass/open_vlm_leaderboard/discussions/7</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/OpenGVLab/MVBench_Leaderboard/discussions/3</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/OpenGVLab/MVBench_Leaderboard/discussions/4</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/openskyml/diffusion-models-leaderboard-template/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/osanseviero/llama-leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/ought/raft-leaderboard/discussions/21</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/patrickvonplaten/parti-prompts-leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/platzi/platzi-leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/PlixAI/pixel-subnet-leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/pngwn/open_llm_leaderboard_two/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/pngwn/open_llm_leaderboard-check/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/pngwn/open_llm_leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/RaoFoundation/pretraining-leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/reach-vb/leaderboards/discussions/4</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/rodrigomasini/data_only_enterprise_scenarios_leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/rodrigomasini/data_only_hallucination_leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/rodrigomasini/data_only_llm_perf_leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/rodrigomasini/data_only_open_llm_leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/rodrigomasini/data-only-mteb-leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/rusticluftig/9-leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/sanchit-gandhi/leaderboards/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/seikwan/open_llm_leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/SIGGRAPH2022/Leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/smothiki/open_llm_leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/smothiki/open_llm_leaderboard2/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/somosnlp/likes_leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/sparse-generative-ai/open-moe-llm-leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/speakleash/open_pl_llm_leaderboard/discussions/4</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/speech-recognition-community-v2/Leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/stabletoolbench/Stable_Tool_Bench_Leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/starmorph/open_llm_leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/stemdataset/stem-leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/ThomasSimonini/Deep-Reinforcement-Learning-Leaderboard-test/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/ThomasSimonini/Deep-Reinforcement-Learning-Leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/ucla-contextual/contextual_leaderboard/discussions/3</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/umdclip/advcalibration/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/upstage/open-ko-llm-leaderboard/discussions/93</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/valory/olas-prediction-leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/vietgpt/VLLMs-Leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/winglian/finetuning_subnet_leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/xtreme-s/leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/yanirmr/hebrew-ASR-leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/ybjeong/leaderboard_kr/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/yhavinga/dutch-tokenizer-arena/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/yzeng58/CoBSAT_Leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/zhangzw16/ProbTS_leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>Uncategorized</t>
+  </si>
+  <si>
+    <t>https://github.com/CLUEbenchmark/SuperCLUE-Safety/issues/5</t>
+  </si>
+  <si>
+    <t>https://github.com/Exploration-Lab/BookSQL/issues/4</t>
+  </si>
+  <si>
+    <t>https://github.com/open-compass/MathBench/issues/4</t>
+  </si>
+  <si>
+    <t>https://github.com/open-compass/MathBench/issues/5</t>
+  </si>
+  <si>
+    <t>https://github.com/OpenGVLab/Multi-Modality-Arena/issues/27</t>
+  </si>
+  <si>
     <t>https://github.com/paperswithcode/paperswithcode-client/issues/24</t>
   </si>
   <si>
-    <t>https://github.com/thu-coai/Safety-Prompts/issues/23</t>
-  </si>
-  <si>
-    <t>https://github.com/whoops-benchmark/whoops-benchmark.github.io/issues/1</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/25</t>
-  </si>
-  <si>
-    <t>https://github.com/stanford-crfm/helm/issues/2205</t>
-  </si>
-  <si>
-    <t>https://github.com/CLUEbenchmark/SuperCLUE/issues/41</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/26</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/mlabonne/Yet_Another_LLM_Leaderboard/discussions/8</t>
-  </si>
-  <si>
-    <t>https://github.com/Q-Future/Q-Bench/issues/11</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/27</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/bhaskartripathi/llm_leaderboards360/discussions/2</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/28</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/29</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/onekq-ai/WebApp1K-models-leaderboard/discussions/2</t>
-  </si>
-  <si>
-    <t>https://github.com/stanford-crfm/helm/issues/2034</t>
-  </si>
-  <si>
-    <t>https://github.com/LudwigStumpp/llm-leaderboard/issues/9</t>
-  </si>
-  <si>
-    <t>https://github.com/embeddings-benchmark/mteb/issues/191</t>
-  </si>
-  <si>
-    <t>https://github.com/LudwigStumpp/llm-leaderboard/issues/10</t>
-  </si>
-  <si>
-    <t>https://github.com/flageval-baai/FlagEval/issues/34</t>
-  </si>
-  <si>
-    <t>https://github.com/stanford-crfm/helm/issues/2060</t>
-  </si>
-  <si>
-    <t>https://github.com/OpenGVLab/Multi-Modality-Arena/issues/25</t>
-  </si>
-  <si>
-    <t>https://github.com/flageval-baai/FlagEval/issues/35</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/32</t>
-  </si>
-  <si>
-    <t>https://github.com/THU-KEG/KoLA/issues/8</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/38</t>
-  </si>
-  <si>
-    <t>https://web.archive.org/web/20221205184917/https://paperswithcode.com/sota/image-classification-on-humaneval</t>
-  </si>
-  <si>
-    <t>https://github.com/Q-Future/Chinese-Q-Bench/issues/2</t>
-  </si>
-  <si>
-    <t>https://web.archive.org/web/20240222011501/https://paperswithcode.com/sota/text-generation-on-humaneval</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/mlabonne/Yet_Another_LLM_Leaderboard/discussions/11</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/speakleash/open_pl_llm_leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://github.com/stanford-crfm/helm/issues/2062</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/41</t>
-  </si>
-  <si>
-    <t>https://github.com/THU-KEG/KoLA/issues/6</t>
-  </si>
-  <si>
-    <t>https://github.com/stanford-crfm/helm/issues/2351</t>
-  </si>
-  <si>
-    <t>https://github.com/stanford-crfm/helm/issues/2239</t>
-  </si>
-  <si>
-    <t>https://github.com/stanford-crfm/helm/issues/2176</t>
-  </si>
-  <si>
-    <t>https://github.com/THU-KEG/KoLA/issues/7</t>
-  </si>
-  <si>
-    <t>https://github.com/THU-KEG/KoLA/issues/2</t>
-  </si>
-  <si>
-    <t>https://github.com/THU-KEG/KoLA/issues/5</t>
-  </si>
-  <si>
-    <t>https://github.com/CLUEbenchmark/SuperCLUE-Code3/issues/2</t>
-  </si>
-  <si>
-    <t>https://github.com/open-compass/LawBench/issues/7</t>
-  </si>
-  <si>
-    <t>https://github.com/msamwelmollel/Swahili_LLM_Leaderboard/issues/2</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/upstage/open-ko-llm-leaderboard/discussions/28</t>
-  </si>
-  <si>
-    <t>https://github.com/jeinlee1991/chinese-llm-benchmark/issues/19</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/30</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/100</t>
-  </si>
-  <si>
-    <t>https://github.com/open-compass/opencompass/discussions/784</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/31</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/101</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/opencompass/open_vlm_leaderboard/discussions/3</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/33</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/102</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/opencompass/open_vlm_leaderboard/discussions/4</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/34</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/103</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/opencompass/open_vlm_leaderboard/discussions/5</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/35</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/104</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/TwinDoc/leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/36</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/105</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/37</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/106</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/mii-llm/open_ita_llm_leaderboard/discussions/4</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/40</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/107</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/valory/olas-prediction-leaderboard/discussions/3</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/42</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/108</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/43</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/109</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/44</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/110</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/45</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/111</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/46</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/112</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/47</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/113</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/48</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/114</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/49</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/115</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/50</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/116</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/52</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/117</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/53</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/118</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/54</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/119</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/55</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/120</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/56</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/121</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/57</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/122</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/58</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/123</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/59</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/124</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/60</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/125</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/61</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/126</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/62</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/127</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/63</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/128</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/64</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/129</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/65</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/130</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/66</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/131</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/67</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/132</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/68</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/133</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/69</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/134</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/70</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/135</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/71</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/136</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/72</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/137</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/73</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/138</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/74</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/139</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/75</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/140</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/76</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/141</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/77</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/142</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/78</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/143</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/79</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/144</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/81</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/145</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/82</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/146</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/83</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/147</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/84</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/148</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/149</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/150</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/151</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/152</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/153</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/154</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/155</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/156</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/157</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/158</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/159</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/160</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/161</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/162</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/163</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/164</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/85</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/86</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/87</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/88</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/89</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/90</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/91</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/92</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/93</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/94</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/95</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/96</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/97</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/98</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/99</t>
-  </si>
-  <si>
-    <t>https://github.com/stanford-crfm/helm/issues/2008</t>
-  </si>
-  <si>
-    <t>https://github.com/stanford-crfm/helm/issues/2010</t>
-  </si>
-  <si>
-    <t>https://github.com/THU-KEG/KoLA/issues/18</t>
-  </si>
-  <si>
-    <t>https://github.com/tjunlp-lab/Awesome-LLMs-Evaluation-Papers/issues/27</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/instructkr/ko-chatbot-arena-leaderboard/discussions/4</t>
-  </si>
-  <si>
-    <t>https://github.com/OpenGVLab/Multi-Modality-Arena/issues/26</t>
-  </si>
-  <si>
-    <t>https://github.com/THU-KEG/KoLA/issues/17</t>
-  </si>
-  <si>
-    <t>https://github.com/flageval-baai/FlagEval/issues/36</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/archit11/Hindi_LLM_arena/discussions/1</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/39</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/cambioml/parser-leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://github.com/stanford-crfm/helm/issues/2039</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/instructkr/ko-chatbot-arena-leaderboard/discussions/5</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/0x1668/open_llm_leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/NexaAIDev/domain_llm_leaderboard/discussions/4</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/0x9/finetuning_subnet_leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/0x9/pretraining-leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/Aarifkhan/leaderboard-results-to-modelcard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/abidlabs/chatbot-arena-leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/abidlabs/mteb-leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/AI-Vietnam/prompt-translation-vie-leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/aichampions/open_llm_leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/Alfasign/open_llm_leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/anglesplato/Deep-Reinforcement-Learning-Leaderboard-V2/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/anirudh937/open_llm_leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/arshy/leaderboard-docker/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/arshy/leaderboard-gradio/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/arshy/leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/asir0z/open_llm_leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/autogenCTF/agent_ctf_leaderboard/discussions/3</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/automerger/Yet_Another_LLM_Leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/awacke1/CanAICode-Leaderboard-Customized/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/b1sheng/kg_llm_leaderboard_test/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/BioMed-VITAL/leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/bittensor-dataset/leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/CathieDaDa/LLM_leaderboard/discussions/3</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/CDT-BMAI-GP/biomed_probing_leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/choco9966/open-ko-llm-leaderboard-old/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/Classroom-workshop/assignments-leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/crynux-ai/genki-dama-leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/CVPR/Leaderboard/discussions/2</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/DeepBrainz/open_llm_leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/deepcode-ai/deepcode-models-leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/demo-crafters/leaderboard/discussions/2</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/demo-leaderboard-backend/leaderboard/discussions/6</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/deprem-ml/intent-leaderboard-v13/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/deprem-ml/intent-leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/dimbyTa/open-llm-leaderboard-viz/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/Docfile/open_llm_leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/DontPlanToEnd/UGI-Leaderboard/discussions/4</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/ECCV2022/Leaderboard/discussions/2</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/esb/leaderboard/discussions/3</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/EuroPython2022/Leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/EuroSciPy2022/Leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/felixz/open_llm_leaderboard/discussions/2</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/freddyaboulton/gradio_leaderboard_demo/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/gblazex/leaderboard/discussions/5</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/gsaivinay/open_llm_leaderboard/discussions/4</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/gsaivinay/open_llm_leaderboard/discussions/5</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/hjzhou/chatbot-arena-leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/homunculus/Deep-Reinforcement-Learning-Leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/hubistrauss/princeton_benchmarks_leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/HuggingFaceH4/human_eval_llm_leaderboard/discussions/4</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/hugginglearners/Hearts_Leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/ICML2022/Leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/Infin/sn32-testnet-leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/JarvisKi/Stable_Tool_Bench_Leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/junior-labs/llm-colosseum/discussions/2</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/k8si/mteb_leaderboard_mtr/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/kbmlcoding/open_llm_leaderboard_free/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/kevinwang676/ocrbench-leaderboard/discussions/2</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/khhuiyh/AutoEval-Video_LeaderBoard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/Koshti10/leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/ludwigstumpp/llm-leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/macrocosm-os/finetuning-leaderboard/discussions/3</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/macrocosm-os/pretraining-leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/Manavshah/dippy-leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/mesolitica/malaysian-stt-leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/MIMIC-CDM/leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/mlfoundations/VisIT-Bench-Leaderboard/discussions/2</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/MohamedRashad/timm-leaderboard/discussions/2</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/Mollel/swahili-llm-leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/NAACL2022/Spaces-Leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/nan/leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/neelalex/leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/nlphuji/WHOOPS-Leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/nouamanetazi/mteb-leaderboard-old/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/Nymbo/leaderboard_main/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/opencompass/open_vlm_leaderboard/discussions/7</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/OpenGVLab/MVBench_Leaderboard/discussions/3</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/OpenGVLab/MVBench_Leaderboard/discussions/4</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/openskyml/diffusion-models-leaderboard-template/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/osanseviero/llama-leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/ought/raft-leaderboard/discussions/21</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/patrickvonplaten/parti-prompts-leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/platzi/platzi-leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/PlixAI/pixel-subnet-leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/pngwn/open_llm_leaderboard_two/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/pngwn/open_llm_leaderboard-check/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/pngwn/open_llm_leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/RaoFoundation/pretraining-leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/reach-vb/leaderboards/discussions/4</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/rodrigomasini/data_only_enterprise_scenarios_leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/rodrigomasini/data_only_hallucination_leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/rodrigomasini/data_only_llm_perf_leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/rodrigomasini/data_only_open_llm_leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/rodrigomasini/data-only-mteb-leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/rusticluftig/9-leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/sanchit-gandhi/leaderboards/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/seikwan/open_llm_leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/SIGGRAPH2022/Leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/smothiki/open_llm_leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/smothiki/open_llm_leaderboard2/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/somosnlp/likes_leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/sparse-generative-ai/open-moe-llm-leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/speakleash/open_pl_llm_leaderboard/discussions/4</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/speech-recognition-community-v2/Leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/stabletoolbench/Stable_Tool_Bench_Leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/starmorph/open_llm_leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/stemdataset/stem-leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/ThomasSimonini/Deep-Reinforcement-Learning-Leaderboard-test/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/ThomasSimonini/Deep-Reinforcement-Learning-Leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/ucla-contextual/contextual_leaderboard/discussions/3</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/umdclip/advcalibration/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/upstage/open-ko-llm-leaderboard/discussions/93</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/valory/olas-prediction-leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/vietgpt/VLLMs-Leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/winglian/finetuning_subnet_leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/xtreme-s/leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/yanirmr/hebrew-ASR-leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/ybjeong/leaderboard_kr/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/yhavinga/dutch-tokenizer-arena/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/yzeng58/CoBSAT_Leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/zhangzw16/ProbTS_leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>Uncategorized</t>
-  </si>
-  <si>
-    <t>https://github.com/CLUEbenchmark/SuperCLUE-Safety/issues/5</t>
-  </si>
-  <si>
-    <t>https://github.com/Exploration-Lab/BookSQL/issues/4</t>
-  </si>
-  <si>
-    <t>https://github.com/open-compass/MathBench/issues/4</t>
-  </si>
-  <si>
-    <t>https://github.com/open-compass/MathBench/issues/5</t>
-  </si>
-  <si>
-    <t>https://github.com/OpenGVLab/Multi-Modality-Arena/issues/27</t>
-  </si>
-  <si>
-    <t>https://github.com/paperswithcode/sota-extractor/issues/80</t>
-  </si>
-  <si>
     <t>https://github.com/TabbyML/tabby/discussions/1368</t>
   </si>
   <si>
@@ -8418,6 +8418,9 @@
     <t>https://huggingface.co/spaces/abhijeethp/embedding_arena/discussions/2</t>
   </si>
   <si>
+    <t>https://huggingface.co/spaces/abhijeethp/embedding_arena/discussions/5</t>
+  </si>
+  <si>
     <t>https://huggingface.co/spaces/CathieDaDa/LLM_leaderboard/discussions/2</t>
   </si>
   <si>
@@ -8440,16 +8443,13 @@
   </si>
   <si>
     <t>https://huggingface.co/spaces/TwinDoc/leaderboard/discussions/2</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/abhijeethp/embedding_arena/discussions/5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="85">
+  <fonts count="84">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -8853,7 +8853,6 @@
       <name val="Roboto"/>
     </font>
     <font>
-      <b/>
       <u/>
       <color rgb="FF0000FF"/>
       <name val="Roboto"/>
@@ -8865,11 +8864,7 @@
       <name val="Roboto"/>
     </font>
     <font>
-      <u/>
-      <color rgb="FF0000FF"/>
-      <name val="Roboto"/>
-    </font>
-    <font>
+      <b/>
       <u/>
       <color rgb="FF0000FF"/>
       <name val="Roboto"/>
@@ -9398,7 +9393,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="147">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -9823,10 +9818,10 @@
     <xf borderId="30" fillId="3" fontId="78" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="29" fillId="2" fontId="79" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="30" fillId="3" fontId="79" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="30" fillId="3" fontId="80" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="29" fillId="2" fontId="80" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="32" fillId="4" fontId="81" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -9835,10 +9830,7 @@
     <xf borderId="33" fillId="0" fontId="82" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="33" fillId="0" fontId="83" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="34" fillId="0" fontId="84" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="34" fillId="0" fontId="83" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -10050,7 +10042,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I19" displayName="Table4" name="Table4" id="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I18" displayName="Table4" name="Table4" id="4">
   <tableColumns count="9">
     <tableColumn name="Benchmark Metric" id="1"/>
     <tableColumn name="Benchmark Protocol" id="2"/>
@@ -23634,7 +23626,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="139" t="s">
+      <c r="A14" s="141" t="s">
         <v>1372</v>
       </c>
     </row>
@@ -23644,17 +23636,17 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="141" t="s">
+      <c r="A16" s="142" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="142" t="s">
+      <c r="A17" s="143" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="143" t="s">
+      <c r="A18" s="141" t="s">
         <v>1373</v>
       </c>
     </row>
@@ -23674,37 +23666,37 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="141" t="s">
+      <c r="A22" s="142" t="s">
         <v>1377</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="136" t="s">
+      <c r="A23" s="138" t="s">
         <v>1378</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="145" t="s">
+      <c r="A24" s="136" t="s">
+        <v>1379</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="140" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="141" t="s">
-        <v>1379</v>
-      </c>
-    </row>
     <row r="26">
-      <c r="A26" s="146" t="s">
+      <c r="A26" s="142" t="s">
         <v>1380</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="136" t="s">
+      <c r="A27" s="138" t="s">
         <v>1381</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="134" t="s">
+      <c r="A28" s="136" t="s">
         <v>1382</v>
       </c>
     </row>
@@ -23715,60 +23707,60 @@
     </row>
     <row r="30">
       <c r="A30" s="134" t="s">
+        <v>1384</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="134" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" s="142" t="s">
+    <row r="32">
+      <c r="A32" s="143" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" s="142" t="s">
-        <v>1384</v>
-      </c>
-    </row>
     <row r="33">
-      <c r="A33" s="140" t="s">
+      <c r="A33" s="143" t="s">
         <v>1385</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="139" t="s">
-        <v>215</v>
+      <c r="A34" s="145" t="s">
+        <v>1386</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="139" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="139" t="s">
         <v>997</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" s="142" t="s">
+    <row r="37">
+      <c r="A37" s="143" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" s="138" t="s">
+    <row r="38">
+      <c r="A38" s="146" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" s="147" t="s">
-        <v>1386</v>
-      </c>
+    <row r="58">
+      <c r="A58" s="80"/>
     </row>
     <row r="59">
       <c r="A59" s="80"/>
     </row>
-    <row r="60">
-      <c r="A60" s="80"/>
+    <row r="61">
+      <c r="A61" s="80"/>
     </row>
     <row r="62">
       <c r="A62" s="80"/>
-    </row>
-    <row r="63">
-      <c r="A63" s="80"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -24379,61 +24371,56 @@
     </row>
     <row r="9">
       <c r="H9" s="64" t="s">
-        <v>1052</v>
+        <v>882</v>
       </c>
     </row>
     <row r="10">
       <c r="H10" s="64" t="s">
-        <v>882</v>
+        <v>660</v>
       </c>
     </row>
     <row r="11">
       <c r="H11" s="64" t="s">
-        <v>660</v>
+        <v>775</v>
       </c>
     </row>
     <row r="12">
-      <c r="H12" s="64" t="s">
-        <v>775</v>
+      <c r="H12" s="16" t="s">
+        <v>1052</v>
       </c>
     </row>
     <row r="13">
-      <c r="H13" s="75" t="s">
+      <c r="H13" s="64" t="s">
         <v>1053</v>
       </c>
     </row>
     <row r="14">
       <c r="H14" s="64" t="s">
-        <v>1054</v>
+        <v>639</v>
       </c>
     </row>
     <row r="15">
-      <c r="H15" s="64" t="s">
-        <v>639</v>
+      <c r="H15" s="71" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="16">
       <c r="H16" s="71" t="s">
-        <v>130</v>
+        <v>604</v>
       </c>
     </row>
     <row r="17">
-      <c r="H17" s="71" t="s">
-        <v>604</v>
+      <c r="H17" s="64" t="s">
+        <v>790</v>
       </c>
     </row>
     <row r="18">
-      <c r="H18" s="64" t="s">
-        <v>790</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="H19" s="89" t="s">
+      <c r="H18" s="89" t="s">
         <v>877</v>
       </c>
     </row>
-    <row r="37">
-      <c r="C37" s="80"/>
+    <row r="36">
+      <c r="C36" s="80"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -24466,11 +24453,10 @@
     <hyperlink r:id="rId27" ref="H16"/>
     <hyperlink r:id="rId28" ref="H17"/>
     <hyperlink r:id="rId29" ref="H18"/>
-    <hyperlink r:id="rId30" ref="H19"/>
   </hyperlinks>
-  <drawing r:id="rId31"/>
+  <drawing r:id="rId30"/>
   <tableParts count="1">
-    <tablePart r:id="rId33"/>
+    <tablePart r:id="rId32"/>
   </tableParts>
 </worksheet>
 </file>
@@ -24528,16 +24514,16 @@
     </row>
     <row r="2">
       <c r="A2" s="90" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B2" s="66" t="s">
         <v>1055</v>
-      </c>
-      <c r="B2" s="66" t="s">
-        <v>1056</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="71" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="G2" s="41"/>
       <c r="H2" s="71" t="s">
@@ -24546,10 +24532,10 @@
     </row>
     <row r="3">
       <c r="A3" s="90" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B3" s="64" t="s">
         <v>1058</v>
-      </c>
-      <c r="B3" s="64" t="s">
-        <v>1059</v>
       </c>
       <c r="E3" s="91"/>
       <c r="F3" s="77" t="s">
@@ -24557,23 +24543,23 @@
       </c>
       <c r="G3" s="70"/>
       <c r="H3" s="64" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="90" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="E4" s="41"/>
       <c r="F4" s="41"/>
       <c r="G4" s="41"/>
       <c r="H4" s="66" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="92" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="E5" s="70"/>
       <c r="F5" s="70"/>
@@ -24584,7 +24570,7 @@
     </row>
     <row r="6">
       <c r="A6" s="90" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
@@ -24596,7 +24582,7 @@
       <c r="E7" s="93"/>
       <c r="F7" s="93"/>
       <c r="H7" s="94" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
   </sheetData>
@@ -24694,23 +24680,23 @@
     </row>
     <row r="2">
       <c r="A2" s="98" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B2" s="99" t="s">
         <v>1066</v>
       </c>
-      <c r="B2" s="99" t="s">
+      <c r="C2" s="100" t="s">
         <v>1067</v>
-      </c>
-      <c r="C2" s="100" t="s">
-        <v>1068</v>
       </c>
       <c r="D2" s="99" t="s">
         <v>116</v>
       </c>
       <c r="E2" s="101"/>
       <c r="F2" s="99" t="s">
+        <v>1068</v>
+      </c>
+      <c r="G2" s="100" t="s">
         <v>1069</v>
-      </c>
-      <c r="G2" s="100" t="s">
-        <v>1070</v>
       </c>
       <c r="H2" s="102" t="s">
         <v>327</v>
@@ -24739,23 +24725,23 @@
     </row>
     <row r="3">
       <c r="A3" s="104" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B3" s="69" t="s">
         <v>1071</v>
       </c>
-      <c r="B3" s="69" t="s">
+      <c r="C3" s="64" t="s">
         <v>1072</v>
-      </c>
-      <c r="C3" s="64" t="s">
-        <v>1073</v>
       </c>
       <c r="D3" s="64" t="s">
         <v>459</v>
       </c>
       <c r="E3" s="70"/>
       <c r="F3" s="75" t="s">
+        <v>1073</v>
+      </c>
+      <c r="G3" s="100" t="s">
         <v>1074</v>
-      </c>
-      <c r="G3" s="100" t="s">
-        <v>1075</v>
       </c>
       <c r="I3" s="105"/>
       <c r="J3" s="97"/>
@@ -24785,7 +24771,7 @@
       </c>
       <c r="E4" s="41"/>
       <c r="F4" s="16" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="G4" s="65" t="s">
         <v>336</v>
@@ -24815,11 +24801,11 @@
     <row r="5">
       <c r="C5" s="106"/>
       <c r="D5" s="100" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="E5" s="91"/>
       <c r="F5" s="69" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="G5" s="107" t="s">
         <v>546</v>
@@ -24850,14 +24836,14 @@
     <row r="6">
       <c r="C6" s="109"/>
       <c r="D6" s="110" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="E6" s="109"/>
       <c r="F6" s="110" t="s">
+        <v>1079</v>
+      </c>
+      <c r="G6" s="111" t="s">
         <v>1080</v>
-      </c>
-      <c r="G6" s="111" t="s">
-        <v>1081</v>
       </c>
       <c r="H6" s="112"/>
       <c r="I6" s="113"/>
@@ -55719,38 +55705,38 @@
       <c r="A2" s="81"/>
       <c r="B2" s="7"/>
       <c r="D2" s="66" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="E2" s="41"/>
       <c r="F2" s="16" t="s">
+        <v>1082</v>
+      </c>
+      <c r="G2" s="64" t="s">
         <v>1083</v>
       </c>
-      <c r="G2" s="64" t="s">
+      <c r="H2" s="82" t="s">
         <v>1084</v>
-      </c>
-      <c r="H2" s="82" t="s">
-        <v>1085</v>
       </c>
     </row>
     <row r="3">
       <c r="D3" s="66" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="E3" s="91"/>
       <c r="F3" s="69" t="s">
+        <v>1086</v>
+      </c>
+      <c r="G3" s="71" t="s">
         <v>1087</v>
       </c>
-      <c r="G3" s="71" t="s">
+      <c r="H3" s="64" t="s">
         <v>1088</v>
-      </c>
-      <c r="H3" s="64" t="s">
-        <v>1089</v>
       </c>
     </row>
     <row r="4">
       <c r="D4" s="115"/>
       <c r="H4" s="110" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="5">
@@ -55831,7 +55817,7 @@
         <v>431</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>523</v>
@@ -55842,10 +55828,10 @@
         <v>994</v>
       </c>
       <c r="G2" s="64" t="s">
+        <v>1091</v>
+      </c>
+      <c r="H2" s="102" t="s">
         <v>1092</v>
-      </c>
-      <c r="H2" s="102" t="s">
-        <v>1093</v>
       </c>
       <c r="I2" s="67" t="s">
         <v>169</v>
@@ -55853,10 +55839,10 @@
     </row>
     <row r="3">
       <c r="A3" s="116" t="s">
+        <v>1093</v>
+      </c>
+      <c r="B3" s="69" t="s">
         <v>1094</v>
-      </c>
-      <c r="B3" s="69" t="s">
-        <v>1095</v>
       </c>
       <c r="C3" s="91"/>
       <c r="D3" s="91"/>
@@ -55865,10 +55851,10 @@
         <v>1018</v>
       </c>
       <c r="G3" s="75" t="s">
+        <v>1095</v>
+      </c>
+      <c r="H3" s="64" t="s">
         <v>1096</v>
-      </c>
-      <c r="H3" s="64" t="s">
-        <v>1097</v>
       </c>
       <c r="I3" s="86" t="s">
         <v>259</v>
@@ -55876,7 +55862,7 @@
     </row>
     <row r="4">
       <c r="B4" s="71" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -55885,10 +55871,10 @@
         <v>621</v>
       </c>
       <c r="G4" s="16" t="s">
+        <v>1098</v>
+      </c>
+      <c r="H4" s="34" t="s">
         <v>1099</v>
-      </c>
-      <c r="H4" s="34" t="s">
-        <v>1100</v>
       </c>
       <c r="I4" s="72" t="s">
         <v>551</v>
@@ -55903,13 +55889,13 @@
       <c r="D5" s="91"/>
       <c r="E5" s="70"/>
       <c r="F5" s="64" t="s">
+        <v>1100</v>
+      </c>
+      <c r="G5" s="75" t="s">
         <v>1101</v>
       </c>
-      <c r="G5" s="75" t="s">
+      <c r="H5" s="69" t="s">
         <v>1102</v>
-      </c>
-      <c r="H5" s="69" t="s">
-        <v>1103</v>
       </c>
       <c r="I5" s="86" t="s">
         <v>566</v>
@@ -55921,13 +55907,13 @@
       <c r="D6" s="41"/>
       <c r="E6" s="41"/>
       <c r="F6" s="64" t="s">
+        <v>1103</v>
+      </c>
+      <c r="G6" s="16" t="s">
         <v>1104</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="H6" s="71" t="s">
         <v>1105</v>
-      </c>
-      <c r="H6" s="71" t="s">
-        <v>1106</v>
       </c>
       <c r="I6" s="24" t="s">
         <v>543</v>
@@ -55939,13 +55925,13 @@
       <c r="D7" s="70"/>
       <c r="E7" s="119"/>
       <c r="F7" s="120" t="s">
+        <v>1106</v>
+      </c>
+      <c r="G7" s="69" t="s">
         <v>1107</v>
       </c>
-      <c r="G7" s="69" t="s">
+      <c r="H7" s="75" t="s">
         <v>1108</v>
-      </c>
-      <c r="H7" s="75" t="s">
-        <v>1109</v>
       </c>
       <c r="I7" s="121" t="s">
         <v>750</v>
@@ -55958,13 +55944,13 @@
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="34" t="s">
+        <v>1109</v>
+      </c>
+      <c r="G8" s="16" t="s">
         <v>1110</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="H8" s="16" t="s">
         <v>1111</v>
-      </c>
-      <c r="H8" s="16" t="s">
-        <v>1112</v>
       </c>
       <c r="I8" s="87" t="s">
         <v>48</v>
@@ -55976,13 +55962,13 @@
       <c r="E9" s="91"/>
       <c r="F9" s="91"/>
       <c r="G9" s="75" t="s">
+        <v>1112</v>
+      </c>
+      <c r="H9" s="64" t="s">
         <v>1113</v>
       </c>
-      <c r="H9" s="64" t="s">
+      <c r="I9" s="86" t="s">
         <v>1114</v>
-      </c>
-      <c r="I9" s="86" t="s">
-        <v>1115</v>
       </c>
     </row>
     <row r="10">
@@ -55992,13 +55978,13 @@
       <c r="E10" s="41"/>
       <c r="F10" s="41"/>
       <c r="G10" s="16" t="s">
+        <v>1115</v>
+      </c>
+      <c r="H10" s="71" t="s">
         <v>1116</v>
       </c>
-      <c r="H10" s="71" t="s">
+      <c r="I10" s="86" t="s">
         <v>1117</v>
-      </c>
-      <c r="I10" s="86" t="s">
-        <v>1118</v>
       </c>
     </row>
     <row r="11">
@@ -56006,10 +55992,10 @@
       <c r="E11" s="70"/>
       <c r="F11" s="70"/>
       <c r="G11" s="69" t="s">
+        <v>1118</v>
+      </c>
+      <c r="H11" s="64" t="s">
         <v>1119</v>
-      </c>
-      <c r="H11" s="64" t="s">
-        <v>1120</v>
       </c>
       <c r="I11" s="78" t="s">
         <v>669</v>
@@ -56022,10 +56008,10 @@
       <c r="E12" s="41"/>
       <c r="F12" s="41"/>
       <c r="G12" s="16" t="s">
+        <v>1120</v>
+      </c>
+      <c r="H12" s="64" t="s">
         <v>1121</v>
-      </c>
-      <c r="H12" s="64" t="s">
-        <v>1122</v>
       </c>
     </row>
     <row r="13">
@@ -56035,10 +56021,10 @@
       <c r="E13" s="70"/>
       <c r="F13" s="70"/>
       <c r="G13" s="69" t="s">
+        <v>1122</v>
+      </c>
+      <c r="H13" s="64" t="s">
         <v>1123</v>
-      </c>
-      <c r="H13" s="64" t="s">
-        <v>1124</v>
       </c>
     </row>
     <row r="14">
@@ -56048,10 +56034,10 @@
       <c r="E14" s="41"/>
       <c r="F14" s="41"/>
       <c r="G14" s="16" t="s">
+        <v>1124</v>
+      </c>
+      <c r="H14" s="16" t="s">
         <v>1125</v>
-      </c>
-      <c r="H14" s="16" t="s">
-        <v>1126</v>
       </c>
     </row>
     <row r="15">
@@ -56061,10 +56047,10 @@
       <c r="E15" s="70"/>
       <c r="F15" s="70"/>
       <c r="G15" s="69" t="s">
+        <v>1126</v>
+      </c>
+      <c r="H15" s="64" t="s">
         <v>1127</v>
-      </c>
-      <c r="H15" s="64" t="s">
-        <v>1128</v>
       </c>
     </row>
     <row r="16">
@@ -56074,10 +56060,10 @@
       <c r="E16" s="41"/>
       <c r="F16" s="41"/>
       <c r="G16" s="34" t="s">
+        <v>1128</v>
+      </c>
+      <c r="H16" s="64" t="s">
         <v>1129</v>
-      </c>
-      <c r="H16" s="64" t="s">
-        <v>1130</v>
       </c>
     </row>
     <row r="17">
@@ -56087,10 +56073,10 @@
       <c r="E17" s="70"/>
       <c r="F17" s="70"/>
       <c r="G17" s="75" t="s">
+        <v>1130</v>
+      </c>
+      <c r="H17" s="64" t="s">
         <v>1131</v>
-      </c>
-      <c r="H17" s="64" t="s">
-        <v>1132</v>
       </c>
     </row>
     <row r="18">
@@ -56100,10 +56086,10 @@
       <c r="E18" s="41"/>
       <c r="F18" s="41"/>
       <c r="G18" s="16" t="s">
+        <v>1132</v>
+      </c>
+      <c r="H18" s="64" t="s">
         <v>1133</v>
-      </c>
-      <c r="H18" s="64" t="s">
-        <v>1134</v>
       </c>
     </row>
     <row r="19">
@@ -56113,10 +56099,10 @@
       <c r="E19" s="70"/>
       <c r="F19" s="70"/>
       <c r="G19" s="69" t="s">
+        <v>1134</v>
+      </c>
+      <c r="H19" s="64" t="s">
         <v>1135</v>
-      </c>
-      <c r="H19" s="64" t="s">
-        <v>1136</v>
       </c>
     </row>
     <row r="20">
@@ -56126,10 +56112,10 @@
       <c r="E20" s="41"/>
       <c r="F20" s="41"/>
       <c r="G20" s="34" t="s">
+        <v>1136</v>
+      </c>
+      <c r="H20" s="64" t="s">
         <v>1137</v>
-      </c>
-      <c r="H20" s="64" t="s">
-        <v>1138</v>
       </c>
     </row>
     <row r="21">
@@ -56139,10 +56125,10 @@
       <c r="E21" s="70"/>
       <c r="F21" s="70"/>
       <c r="G21" s="69" t="s">
+        <v>1138</v>
+      </c>
+      <c r="H21" s="71" t="s">
         <v>1139</v>
-      </c>
-      <c r="H21" s="71" t="s">
-        <v>1140</v>
       </c>
     </row>
     <row r="22">
@@ -56150,76 +56136,76 @@
       <c r="C22" s="41"/>
       <c r="D22" s="41"/>
       <c r="G22" s="34" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H22" s="64" t="s">
         <v>1141</v>
-      </c>
-      <c r="H22" s="64" t="s">
-        <v>1142</v>
       </c>
     </row>
     <row r="23">
       <c r="G23" s="69" t="s">
+        <v>1142</v>
+      </c>
+      <c r="H23" s="64" t="s">
         <v>1143</v>
-      </c>
-      <c r="H23" s="64" t="s">
-        <v>1144</v>
       </c>
     </row>
     <row r="24">
       <c r="G24" s="34" t="s">
+        <v>1144</v>
+      </c>
+      <c r="H24" s="64" t="s">
         <v>1145</v>
-      </c>
-      <c r="H24" s="64" t="s">
-        <v>1146</v>
       </c>
     </row>
     <row r="25">
       <c r="G25" s="69" t="s">
+        <v>1146</v>
+      </c>
+      <c r="H25" s="69" t="s">
         <v>1147</v>
-      </c>
-      <c r="H25" s="69" t="s">
-        <v>1148</v>
       </c>
     </row>
     <row r="26">
       <c r="G26" s="34" t="s">
+        <v>1148</v>
+      </c>
+      <c r="H26" s="16" t="s">
         <v>1149</v>
-      </c>
-      <c r="H26" s="16" t="s">
-        <v>1150</v>
       </c>
     </row>
     <row r="27">
       <c r="G27" s="69" t="s">
+        <v>1150</v>
+      </c>
+      <c r="H27" s="64" t="s">
         <v>1151</v>
-      </c>
-      <c r="H27" s="64" t="s">
-        <v>1152</v>
       </c>
     </row>
     <row r="28">
       <c r="G28" s="16" t="s">
+        <v>1152</v>
+      </c>
+      <c r="H28" s="64" t="s">
         <v>1153</v>
-      </c>
-      <c r="H28" s="64" t="s">
-        <v>1154</v>
       </c>
     </row>
     <row r="29">
       <c r="G29" s="69" t="s">
+        <v>1154</v>
+      </c>
+      <c r="H29" s="64" t="s">
         <v>1155</v>
-      </c>
-      <c r="H29" s="64" t="s">
-        <v>1156</v>
       </c>
     </row>
     <row r="30">
       <c r="E30" s="41"/>
       <c r="F30" s="41"/>
       <c r="G30" s="34" t="s">
+        <v>1156</v>
+      </c>
+      <c r="H30" s="64" t="s">
         <v>1157</v>
-      </c>
-      <c r="H30" s="64" t="s">
-        <v>1158</v>
       </c>
     </row>
     <row r="31">
@@ -56227,20 +56213,20 @@
       <c r="C31" s="70"/>
       <c r="D31" s="70"/>
       <c r="G31" s="69" t="s">
+        <v>1158</v>
+      </c>
+      <c r="H31" s="71" t="s">
         <v>1159</v>
-      </c>
-      <c r="H31" s="71" t="s">
-        <v>1160</v>
       </c>
     </row>
     <row r="32">
       <c r="E32" s="41"/>
       <c r="F32" s="41"/>
       <c r="G32" s="16" t="s">
+        <v>1160</v>
+      </c>
+      <c r="H32" s="64" t="s">
         <v>1161</v>
-      </c>
-      <c r="H32" s="64" t="s">
-        <v>1162</v>
       </c>
     </row>
     <row r="33">
@@ -56250,10 +56236,10 @@
       <c r="E33" s="70"/>
       <c r="F33" s="70"/>
       <c r="G33" s="69" t="s">
+        <v>1162</v>
+      </c>
+      <c r="H33" s="71" t="s">
         <v>1163</v>
-      </c>
-      <c r="H33" s="71" t="s">
-        <v>1164</v>
       </c>
     </row>
     <row r="34">
@@ -56263,10 +56249,10 @@
       <c r="E34" s="41"/>
       <c r="F34" s="41"/>
       <c r="G34" s="34" t="s">
+        <v>1164</v>
+      </c>
+      <c r="H34" s="71" t="s">
         <v>1165</v>
-      </c>
-      <c r="H34" s="71" t="s">
-        <v>1166</v>
       </c>
     </row>
     <row r="35">
@@ -56274,20 +56260,20 @@
       <c r="C35" s="70"/>
       <c r="D35" s="70"/>
       <c r="G35" s="69" t="s">
+        <v>1166</v>
+      </c>
+      <c r="H35" s="71" t="s">
         <v>1167</v>
-      </c>
-      <c r="H35" s="71" t="s">
-        <v>1168</v>
       </c>
     </row>
     <row r="36">
       <c r="E36" s="41"/>
       <c r="F36" s="41"/>
       <c r="G36" s="16" t="s">
+        <v>1168</v>
+      </c>
+      <c r="H36" s="64" t="s">
         <v>1169</v>
-      </c>
-      <c r="H36" s="64" t="s">
-        <v>1170</v>
       </c>
     </row>
     <row r="37">
@@ -56297,10 +56283,10 @@
       <c r="E37" s="70"/>
       <c r="F37" s="70"/>
       <c r="G37" s="75" t="s">
+        <v>1170</v>
+      </c>
+      <c r="H37" s="64" t="s">
         <v>1171</v>
-      </c>
-      <c r="H37" s="64" t="s">
-        <v>1172</v>
       </c>
     </row>
     <row r="38">
@@ -56308,52 +56294,52 @@
       <c r="C38" s="41"/>
       <c r="D38" s="41"/>
       <c r="G38" s="34" t="s">
+        <v>1172</v>
+      </c>
+      <c r="H38" s="64" t="s">
         <v>1173</v>
-      </c>
-      <c r="H38" s="64" t="s">
-        <v>1174</v>
       </c>
     </row>
     <row r="39">
       <c r="G39" s="75" t="s">
+        <v>1174</v>
+      </c>
+      <c r="H39" s="64" t="s">
         <v>1175</v>
-      </c>
-      <c r="H39" s="64" t="s">
-        <v>1176</v>
       </c>
     </row>
     <row r="40">
       <c r="G40" s="34" t="s">
+        <v>1176</v>
+      </c>
+      <c r="H40" s="64" t="s">
         <v>1177</v>
-      </c>
-      <c r="H40" s="64" t="s">
-        <v>1178</v>
       </c>
     </row>
     <row r="41">
       <c r="G41" s="69" t="s">
+        <v>1178</v>
+      </c>
+      <c r="H41" s="75" t="s">
         <v>1179</v>
-      </c>
-      <c r="H41" s="75" t="s">
-        <v>1180</v>
       </c>
     </row>
     <row r="42">
       <c r="G42" s="34" t="s">
+        <v>1180</v>
+      </c>
+      <c r="H42" s="64" t="s">
         <v>1181</v>
-      </c>
-      <c r="H42" s="64" t="s">
-        <v>1182</v>
       </c>
     </row>
     <row r="43">
       <c r="E43" s="70"/>
       <c r="F43" s="70"/>
       <c r="G43" s="69" t="s">
+        <v>1182</v>
+      </c>
+      <c r="H43" s="69" t="s">
         <v>1183</v>
-      </c>
-      <c r="H43" s="69" t="s">
-        <v>1184</v>
       </c>
     </row>
     <row r="44">
@@ -56363,10 +56349,10 @@
       <c r="E44" s="41"/>
       <c r="F44" s="41"/>
       <c r="G44" s="34" t="s">
+        <v>1184</v>
+      </c>
+      <c r="H44" s="64" t="s">
         <v>1185</v>
-      </c>
-      <c r="H44" s="64" t="s">
-        <v>1186</v>
       </c>
     </row>
     <row r="45">
@@ -56374,20 +56360,20 @@
       <c r="C45" s="70"/>
       <c r="D45" s="70"/>
       <c r="G45" s="69" t="s">
+        <v>1186</v>
+      </c>
+      <c r="H45" s="64" t="s">
         <v>1187</v>
-      </c>
-      <c r="H45" s="64" t="s">
-        <v>1188</v>
       </c>
     </row>
     <row r="46">
       <c r="E46" s="41"/>
       <c r="F46" s="41"/>
       <c r="G46" s="34" t="s">
+        <v>1188</v>
+      </c>
+      <c r="H46" s="71" t="s">
         <v>1189</v>
-      </c>
-      <c r="H46" s="71" t="s">
-        <v>1190</v>
       </c>
     </row>
     <row r="47">
@@ -56395,45 +56381,48 @@
       <c r="C47" s="70"/>
       <c r="D47" s="70"/>
       <c r="G47" s="69" t="s">
+        <v>1190</v>
+      </c>
+      <c r="H47" s="71" t="s">
         <v>1191</v>
       </c>
-      <c r="H47" s="71" t="s">
+    </row>
+    <row r="48">
+      <c r="G48" s="64" t="s">
         <v>1192</v>
       </c>
-    </row>
-    <row r="48">
-      <c r="G48" s="34" t="s">
+      <c r="H48" s="64" t="s">
         <v>1193</v>
-      </c>
-      <c r="H48" s="71" t="s">
-        <v>1194</v>
       </c>
     </row>
     <row r="49">
       <c r="G49" s="69" t="s">
+        <v>1194</v>
+      </c>
+      <c r="H49" s="71" t="s">
         <v>1195</v>
-      </c>
-      <c r="H49" s="64" t="s">
-        <v>1196</v>
       </c>
     </row>
     <row r="50">
       <c r="G50" s="34" t="s">
+        <v>1196</v>
+      </c>
+      <c r="H50" s="64" t="s">
         <v>1197</v>
-      </c>
-      <c r="H50" s="71" t="s">
-        <v>1198</v>
       </c>
     </row>
     <row r="51">
       <c r="G51" s="69" t="s">
+        <v>1198</v>
+      </c>
+      <c r="H51" s="71" t="s">
         <v>1199</v>
       </c>
-      <c r="H51" s="64" t="s">
+    </row>
+    <row r="52">
+      <c r="G52" s="34" t="s">
         <v>1200</v>
       </c>
-    </row>
-    <row r="52">
       <c r="H52" s="64" t="s">
         <v>1201</v>
       </c>
@@ -56759,50 +56748,51 @@
     <hyperlink r:id="rId122" ref="H50"/>
     <hyperlink r:id="rId123" ref="G51"/>
     <hyperlink r:id="rId124" ref="H51"/>
-    <hyperlink r:id="rId125" ref="H52"/>
-    <hyperlink r:id="rId126" ref="H53"/>
-    <hyperlink r:id="rId127" ref="H54"/>
-    <hyperlink r:id="rId128" ref="H55"/>
-    <hyperlink r:id="rId129" ref="H56"/>
-    <hyperlink r:id="rId130" ref="H57"/>
-    <hyperlink r:id="rId131" ref="H58"/>
-    <hyperlink r:id="rId132" ref="H59"/>
-    <hyperlink r:id="rId133" ref="H60"/>
-    <hyperlink r:id="rId134" ref="H61"/>
-    <hyperlink r:id="rId135" ref="H62"/>
-    <hyperlink r:id="rId136" ref="H63"/>
-    <hyperlink r:id="rId137" ref="H64"/>
-    <hyperlink r:id="rId138" ref="H65"/>
-    <hyperlink r:id="rId139" ref="H66"/>
-    <hyperlink r:id="rId140" ref="H67"/>
-    <hyperlink r:id="rId141" ref="H68"/>
-    <hyperlink r:id="rId142" ref="H69"/>
-    <hyperlink r:id="rId143" ref="H70"/>
-    <hyperlink r:id="rId144" ref="H71"/>
-    <hyperlink r:id="rId145" ref="H72"/>
-    <hyperlink r:id="rId146" ref="H73"/>
-    <hyperlink r:id="rId147" ref="H74"/>
-    <hyperlink r:id="rId148" ref="H75"/>
-    <hyperlink r:id="rId149" ref="H76"/>
-    <hyperlink r:id="rId150" ref="H77"/>
-    <hyperlink r:id="rId151" ref="H78"/>
-    <hyperlink r:id="rId152" ref="H79"/>
-    <hyperlink r:id="rId153" ref="H80"/>
-    <hyperlink r:id="rId154" ref="H81"/>
-    <hyperlink r:id="rId155" ref="H82"/>
-    <hyperlink r:id="rId156" ref="H83"/>
-    <hyperlink r:id="rId157" ref="H84"/>
-    <hyperlink r:id="rId158" ref="H85"/>
-    <hyperlink r:id="rId159" ref="H86"/>
-    <hyperlink r:id="rId160" ref="H87"/>
-    <hyperlink r:id="rId161" ref="H88"/>
-    <hyperlink r:id="rId162" ref="H89"/>
-    <hyperlink r:id="rId163" ref="H90"/>
-    <hyperlink r:id="rId164" ref="H91"/>
+    <hyperlink r:id="rId125" ref="G52"/>
+    <hyperlink r:id="rId126" ref="H52"/>
+    <hyperlink r:id="rId127" ref="H53"/>
+    <hyperlink r:id="rId128" ref="H54"/>
+    <hyperlink r:id="rId129" ref="H55"/>
+    <hyperlink r:id="rId130" ref="H56"/>
+    <hyperlink r:id="rId131" ref="H57"/>
+    <hyperlink r:id="rId132" ref="H58"/>
+    <hyperlink r:id="rId133" ref="H59"/>
+    <hyperlink r:id="rId134" ref="H60"/>
+    <hyperlink r:id="rId135" ref="H61"/>
+    <hyperlink r:id="rId136" ref="H62"/>
+    <hyperlink r:id="rId137" ref="H63"/>
+    <hyperlink r:id="rId138" ref="H64"/>
+    <hyperlink r:id="rId139" ref="H65"/>
+    <hyperlink r:id="rId140" ref="H66"/>
+    <hyperlink r:id="rId141" ref="H67"/>
+    <hyperlink r:id="rId142" ref="H68"/>
+    <hyperlink r:id="rId143" ref="H69"/>
+    <hyperlink r:id="rId144" ref="H70"/>
+    <hyperlink r:id="rId145" ref="H71"/>
+    <hyperlink r:id="rId146" ref="H72"/>
+    <hyperlink r:id="rId147" ref="H73"/>
+    <hyperlink r:id="rId148" ref="H74"/>
+    <hyperlink r:id="rId149" ref="H75"/>
+    <hyperlink r:id="rId150" ref="H76"/>
+    <hyperlink r:id="rId151" ref="H77"/>
+    <hyperlink r:id="rId152" ref="H78"/>
+    <hyperlink r:id="rId153" ref="H79"/>
+    <hyperlink r:id="rId154" ref="H80"/>
+    <hyperlink r:id="rId155" ref="H81"/>
+    <hyperlink r:id="rId156" ref="H82"/>
+    <hyperlink r:id="rId157" ref="H83"/>
+    <hyperlink r:id="rId158" ref="H84"/>
+    <hyperlink r:id="rId159" ref="H85"/>
+    <hyperlink r:id="rId160" ref="H86"/>
+    <hyperlink r:id="rId161" ref="H87"/>
+    <hyperlink r:id="rId162" ref="H88"/>
+    <hyperlink r:id="rId163" ref="H89"/>
+    <hyperlink r:id="rId164" ref="H90"/>
+    <hyperlink r:id="rId165" ref="H91"/>
   </hyperlinks>
-  <drawing r:id="rId165"/>
+  <drawing r:id="rId166"/>
   <tableParts count="1">
-    <tablePart r:id="rId167"/>
+    <tablePart r:id="rId168"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
naming tweak of table
</commit_message>
<xml_diff>
--- a/result/Foundation Model Leaderboards.xlsx
+++ b/result/Foundation Model Leaderboards.xlsx
@@ -3664,11 +3664,11 @@
     </comment>
     <comment authorId="0" ref="B1">
       <text>
-        <t xml:space="preserve">ep: Excel platform
-gh: GitHub
+        <t xml:space="preserve">gh: GitHub
 hf: HuggingFace
 ip: independent platform
 pwc: PapersWithCode
+sp: spreadsheet platform
 	-Jimmy Zhao</t>
       </text>
     </comment>
@@ -3861,7 +3861,7 @@
     <t>ai-benchmarks</t>
   </si>
   <si>
-    <t>ep,gh</t>
+    <t>gh,sp</t>
   </si>
   <si>
     <t>https://github.com/fixie-ai/ai-benchmarks</t>
@@ -7131,7 +7131,7 @@
     <t>VisualWebArena</t>
   </si>
   <si>
-    <t>ep,ip</t>
+    <t>ip,sp</t>
   </si>
   <si>
     <t>https://github.com/web-arena-x/visualwebarena</t>
@@ -7189,7 +7189,7 @@
     <t>WebArena</t>
   </si>
   <si>
-    <t>ep</t>
+    <t>sp</t>
   </si>
   <si>
     <t>https://github.com/web-arena-x/webarena</t>
@@ -22550,11 +22550,11 @@
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H2:H809">
       <formula1>"1,1,4,1,4,5,2,2,4,3,4,4,5,5,Workflow patterns,1,5,1,2,4"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="B2:B482">
+      <formula1>"gh,gh,hf,gh,hf,ip,gh,ip,gh,pwc,hf,hf,ip,ip,Host platforms,pwc,gh,sp,sp,ip,sp"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:F809">
       <formula1>"Has any submission channel/protocol?,y"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="B2:B482">
-      <formula1>"gh,gh,hf,gh,hf,ip,gh,ip,gh,pwc,hf,hf,ip,ip,Host platforms,pwc,ep,gh,ep,ep,ip"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E809">
       <formula1>"Attaches model provenance?,y"</formula1>

</xml_diff>